<commit_message>
use our own crc32 logic
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207E5766-F065-4AA4-BA54-74FD8411B1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2D7CCD-EEA1-40F6-9824-D9B03605A45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="1400">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4418,6 +4418,34 @@
   </si>
   <si>
     <t>拖拽面向时实时预览</t>
+  </si>
+  <si>
+    <t>恭喜，您获胜了！\n要再玩一盘吗？</t>
+  </si>
+  <si>
+    <t>EasterEggWin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>胜利！</t>
+  </si>
+  <si>
+    <t>EasterEggWinTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你发现了彩蛋 :-)    按ESC键退出游戏</t>
+  </si>
+  <si>
+    <t>EasterEggDesc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EasterEggTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>彩蛋</t>
   </si>
 </sst>
 </file>
@@ -4799,10 +4827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D725"/>
+  <dimension ref="A1:D729"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A706" workbookViewId="0">
-      <selection activeCell="B720" sqref="B720"/>
+      <selection activeCell="B724" sqref="B724"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10597,6 +10625,38 @@
         <v>1391</v>
       </c>
     </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A726" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B726" s="2" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A727" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B727" s="2" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A728" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B728" s="2" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A729" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B729" s="2" t="s">
+        <v>1399</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix several bugs, change alphaImage drawing order
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2D7CCD-EEA1-40F6-9824-D9B03605A45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E25A750-32CF-42A1-A2A9-6FF31704AA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="1400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="1405">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4446,6 +4446,26 @@
   </si>
   <si>
     <t>彩蛋</t>
+  </si>
+  <si>
+    <t>AI触发</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SearhReference.AITrigger</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SearhReference.Script</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SearhReference.Trigger</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SearhReference.Team</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4827,10 +4847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D729"/>
+  <dimension ref="A1:D733"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A706" workbookViewId="0">
-      <selection activeCell="B724" sqref="B724"/>
+      <selection activeCell="A727" sqref="A727"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10657,6 +10677,38 @@
         <v>1399</v>
       </c>
     </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A730" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B730" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A731" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B731" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A732" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B732" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A733" s="2" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B733" s="2" t="s">
+        <v>1400</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add Chinese chess easter egg, change ini include order to BFS
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E25A750-32CF-42A1-A2A9-6FF31704AA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0530EDF9-919A-4935-B2DC-0EB8888D2274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="1397">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4418,34 +4418,6 @@
   </si>
   <si>
     <t>拖拽面向时实时预览</t>
-  </si>
-  <si>
-    <t>恭喜，您获胜了！\n要再玩一盘吗？</t>
-  </si>
-  <si>
-    <t>EasterEggWin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>胜利！</t>
-  </si>
-  <si>
-    <t>EasterEggWinTitle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你发现了彩蛋 :-)    按ESC键退出游戏</t>
-  </si>
-  <si>
-    <t>EasterEggDesc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EasterEggTitle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>彩蛋</t>
   </si>
   <si>
     <t>AI触发</t>
@@ -4847,10 +4819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D733"/>
+  <dimension ref="A1:D729"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A706" workbookViewId="0">
-      <selection activeCell="A727" sqref="A727"/>
+      <selection activeCell="B724" sqref="B724"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10647,10 +10619,10 @@
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>1393</v>
+        <v>1396</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>1392</v>
+        <v>165</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.3">
@@ -10658,55 +10630,23 @@
         <v>1395</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>1394</v>
+        <v>561</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A728" s="2" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="B728" s="2" t="s">
-        <v>1396</v>
+        <v>573</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A729" s="2" t="s">
-        <v>1398</v>
+        <v>1393</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A730" s="2" t="s">
-        <v>1404</v>
-      </c>
-      <c r="B730" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="731" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A731" s="2" t="s">
-        <v>1403</v>
-      </c>
-      <c r="B731" s="2" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="732" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A732" s="2" t="s">
-        <v>1402</v>
-      </c>
-      <c r="B732" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A733" s="2" t="s">
-        <v>1401</v>
-      </c>
-      <c r="B733" s="2" t="s">
-        <v>1400</v>
+        <v>1392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update chess end game
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3DD519-01D7-4A06-AB64-167FBCD947E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E88395-9B4C-4D3F-AD11-7F9E5D2C2778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3530" yWindow="4570" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="1421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="1425">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4510,6 +4510,22 @@
   </si>
   <si>
     <t>你吃掉了红将！你胜利了！</t>
+  </si>
+  <si>
+    <t>EasterEggChessGameOverMessage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EasterEggChessPlayingMessage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你发现了彩蛋 :-)     按 R 键重新开始，按 Z 键悔棋，按 E 键生成一盘残局</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏结束 - 按 R 键重新开始，按 E 键生成一盘残局</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4891,10 +4907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D741"/>
+  <dimension ref="A1:D743"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A720" workbookViewId="0">
-      <selection activeCell="B725" sqref="B725"/>
+      <selection activeCell="D738" sqref="D738"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10817,6 +10833,22 @@
         <v>1420</v>
       </c>
     </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A742" s="2" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B742" s="2" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A743" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B743" s="2" t="s">
+        <v>1423</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
consider PoweredOn of buildings, optimize drag preview
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E88395-9B4C-4D3F-AD11-7F9E5D2C2778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477BDE1B-6E63-4580-83CA-9F62D362CC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3530" yWindow="4570" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="3890" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="1425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="1427">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4525,6 +4525,14 @@
   </si>
   <si>
     <t>游戏结束 - 按 R 键重新开始，按 E 键生成一盘残局</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ObjectInfo.Structure.7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>血量: %d (%s), 耗能: 0, AI修复: %s</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4907,10 +4915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D743"/>
+  <dimension ref="A1:D744"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A720" workbookViewId="0">
-      <selection activeCell="D738" sqref="D738"/>
+      <selection activeCell="B737" sqref="B737"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10849,6 +10857,14 @@
         <v>1423</v>
       </c>
     </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A744" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B744" s="2" t="s">
+        <v>1426</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rewrite Set overlay data manually window
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477BDE1B-6E63-4580-83CA-9F62D362CC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97C9BFA-33D1-4EC2-B664-3FE49350A6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2850" yWindow="3890" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="1427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="1437">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4533,6 +4533,42 @@
   </si>
   <si>
     <t>血量: %d (%s), 耗能: 0, AI修复: %s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>请输入覆盖物的索引(0-254)，不要超过这个范围。</t>
+  </si>
+  <si>
+    <t>手动设置覆盖物</t>
+  </si>
+  <si>
+    <t>请输入覆盖物的索引(0-65534)，不要超过这个范围。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>请输入覆盖物数据的索引(0-59)，不要超过这个范围。</t>
+  </si>
+  <si>
+    <t>手动设置覆盖物数据</t>
+  </si>
+  <si>
+    <t>ManualOverlayDataTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ManualOverlayDataMessage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ManualOverlayTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ManualOverlayMessageExt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ManualOverlayMessage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4915,10 +4951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D744"/>
+  <dimension ref="A1:D749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A720" workbookViewId="0">
-      <selection activeCell="B737" sqref="B737"/>
+    <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
+      <selection activeCell="B742" sqref="B742"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10865,6 +10901,46 @@
         <v>1426</v>
       </c>
     </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A745" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B745" s="2" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A746" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B746" s="2" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A747" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B747" s="2" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A748" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B748" s="2" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A749" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B749" s="2" t="s">
+        <v>1431</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix Perpetual check issue
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993FA012-7AAF-401A-9765-B4C2EBB84174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8046972-49F5-4EB4-8D63-4723243DC3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="3890" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="3630" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="1441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="1443">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4488,12 +4488,6 @@
     <t>AI被困毙，你胜利了！</t>
   </si>
   <si>
-    <t>EasterEggPerpetualCheck</t>
-  </si>
-  <si>
-    <t>禁止长将，和棋</t>
-  </si>
-  <si>
     <t>EasterEggAICheckMate</t>
   </si>
   <si>
@@ -4584,6 +4578,18 @@
   <si>
     <t>Options.EnableDarkMode.DimMap</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EasterEggAIPerpetualCheckLose</t>
+  </si>
+  <si>
+    <t>禁止长将，你胜利了！</t>
+  </si>
+  <si>
+    <t>EasterEggPlayerPerpetualCheckLose</t>
+  </si>
+  <si>
+    <t>禁止长将，你输了！</t>
   </si>
 </sst>
 </file>
@@ -4965,10 +4971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D751"/>
+  <dimension ref="A1:D752"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
-      <selection activeCell="B742" sqref="B742"/>
+      <selection activeCell="B743" sqref="B743"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10861,114 +10867,122 @@
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A738" s="2" t="s">
-        <v>1413</v>
+        <v>1439</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>1414</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A739" s="2" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A740" s="2" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A741" s="2" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="B741" s="2" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A742" s="2" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="743" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A743" s="2" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A744" s="2" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="B744" s="2" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A745" s="2" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A746" s="2" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A747" s="2" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748" s="2" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A749" s="2" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A750" s="2" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A751" s="2" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1438</v>
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A752" s="2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B752" s="2" t="s">
+        <v>1442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add draw detect & move highlight in gobang
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8046972-49F5-4EB4-8D63-4723243DC3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4F8E51-A841-4F14-9E95-929391EC5B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="3630" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="1443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="1445">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4590,6 +4590,13 @@
   </si>
   <si>
     <t>禁止长将，你输了！</t>
+  </si>
+  <si>
+    <t>EasterEggGoBangDraw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>棋盘已满，和棋！</t>
   </si>
 </sst>
 </file>
@@ -4971,10 +4978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D752"/>
+  <dimension ref="A1:D753"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
-      <selection activeCell="B743" sqref="B743"/>
+      <selection activeCell="B753" sqref="B753"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10985,6 +10992,14 @@
         <v>1442</v>
       </c>
     </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A753" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B753" s="2" t="s">
+        <v>1444</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update shrink tile set browser view image func
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4F8E51-A841-4F14-9E95-929391EC5B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12825BD6-DE49-47B8-8027-7D5C9C94BE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="3630" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="1445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="1447">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4597,6 +4597,13 @@
   </si>
   <si>
     <t>棋盘已满，和棋！</t>
+  </si>
+  <si>
+    <t>Options.ShrinkTilesInTileSetBrowser</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩小地形浏览器的地形图像</t>
   </si>
 </sst>
 </file>
@@ -4978,10 +4985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D753"/>
+  <dimension ref="A1:D754"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
-      <selection activeCell="B753" sqref="B753"/>
+      <selection activeCell="B754" sqref="B754"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11000,6 +11007,14 @@
         <v>1444</v>
       </c>
     </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A754" s="2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B754" s="2" t="s">
+        <v>1446</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjust building anim sorting, add InGameDisplay.AnimAdjust
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12825BD6-DE49-47B8-8027-7D5C9C94BE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CE0412-1F90-4BEF-AAAB-2F864BC01A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="3630" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="1447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="1449">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4604,6 +4604,13 @@
   </si>
   <si>
     <t>缩小地形浏览器的地形图像</t>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.AnimAdjust</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>调节建筑动画图层，可能与游戏内不一致</t>
   </si>
 </sst>
 </file>
@@ -4985,10 +4992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D754"/>
+  <dimension ref="A1:D755"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
-      <selection activeCell="B754" sqref="B754"/>
+      <selection activeCell="B746" sqref="B746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11015,6 +11022,14 @@
         <v>1446</v>
       </c>
     </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A755" s="2" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B755" s="2" t="s">
+        <v>1448</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support death weapon range view
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE3C5B0-740B-442D-8803-88A7A076C71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF30F916-E4D1-4169-874E-CFDF5D549821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="3630" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="1970" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="1451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="1453">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4618,6 +4618,13 @@
   </si>
   <si>
     <t>触发编辑器显示&lt;Player @ X&gt;所属方 (Phobos)</t>
+  </si>
+  <si>
+    <t>ViewDeathWeaponRangeInfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡武器范围</t>
   </si>
 </sst>
 </file>
@@ -4999,10 +5006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D756"/>
+  <dimension ref="A1:D757"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A744" workbookViewId="0">
-      <selection activeCell="B752" sqref="B752"/>
+      <selection activeCell="B757" sqref="B757"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11045,6 +11052,14 @@
         <v>1450</v>
       </c>
     </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A757" s="2" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B757" s="2" t="s">
+        <v>1452</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support palette for all overlays, add missing phobos label
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF30F916-E4D1-4169-874E-CFDF5D549821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86D0ECA-EC09-436B-B18C-4195715ECD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="1970" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15580" yWindow="3010" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3695,12 +3695,6 @@
     <t>地图开头添加编码警告的注释</t>
   </si>
   <si>
-    <t>启用无限路径点 (Phobos)</t>
-  </si>
-  <si>
-    <t>启用无限变量 (Phobos)</t>
-  </si>
-  <si>
     <t>按住shift放置地形时仅记录一次历史</t>
   </si>
   <si>
@@ -3815,9 +3809,6 @@
     <t>加载并显示水中单位的更换图像</t>
   </si>
   <si>
-    <t>加载并显示单位伤残的更换图像 (Phobos)</t>
-  </si>
-  <si>
     <t>将悬浮单位渲染的更高</t>
   </si>
   <si>
@@ -3833,9 +3824,6 @@
     <t>显示地图边界外的游戏对象</t>
   </si>
   <si>
-    <t>单位选项窗口显示&lt;Player @ X&gt;所属方 (Phobos)</t>
-  </si>
-  <si>
     <t>检测地图文件的外部修改</t>
   </si>
   <si>
@@ -4161,10 +4149,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>读取单位art(md).ini中的Image= (Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Options.SortByLabelName.Trigger</t>
   </si>
   <si>
@@ -4226,14 +4210,6 @@
     <t>设置继承类型 (Y = Phobos, N = Ares)</t>
   </si>
   <si>
-    <t>读取#include INI (Ares/Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>允许读取继承的INI小节 (Ares/Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>设置单元格第一个步兵的位置(Y = 4, N = 0)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -4242,10 +4218,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>启用无限覆盖物 (Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>MV_OverlayLimit</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -4617,14 +4589,47 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>触发编辑器显示&lt;Player @ X&gt;所属方 (Phobos)</t>
-  </si>
-  <si>
     <t>ViewDeathWeaponRangeInfo</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>死亡武器范围</t>
+  </si>
+  <si>
+    <t>读取#include INI (Ares/Phobos B34+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取单位art(md).ini中的Image= (Phobos B25+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用无限路径点 (Phobos B16+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用无限变量 (Phobos B22+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加载并显示单位伤残的更换图像 (Phobos B47+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位选项窗口显示&lt;Player @ X&gt;所属方 (Phobos B37+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发编辑器显示&lt;Player @ X&gt;所属方 (Phobos B49+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许读取继承的INI小节 (Ares/Phobos B34+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用无限覆盖物 (Phobos B48+)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5008,8 +5013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A744" workbookViewId="0">
-      <selection activeCell="B757" sqref="B757"/>
+    <sheetView tabSelected="1" topLeftCell="A690" workbookViewId="0">
+      <selection activeCell="B703" sqref="B703"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -6760,7 +6765,7 @@
         <v>411</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>1371</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -6968,7 +6973,7 @@
         <v>462</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1372</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -7248,7 +7253,7 @@
         <v>531</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>1373</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -7488,7 +7493,7 @@
         <v>579</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>1374</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -7568,7 +7573,7 @@
         <v>598</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>1375</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -7576,7 +7581,7 @@
         <v>599</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1376</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -7584,7 +7589,7 @@
         <v>600</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1377</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -7592,7 +7597,7 @@
         <v>601</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>1378</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -7600,7 +7605,7 @@
         <v>602</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>1379</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -7608,7 +7613,7 @@
         <v>603</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>1380</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -7792,7 +7797,7 @@
         <v>644</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>1381</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -8384,7 +8389,7 @@
         <v>779</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1382</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
@@ -9954,7 +9959,7 @@
     </row>
     <row r="620" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A620" s="2" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="B620" s="2" t="s">
         <v>1168</v>
@@ -9962,7 +9967,7 @@
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" s="2" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="B621" s="2" t="s">
         <v>1169</v>
@@ -9970,15 +9975,15 @@
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="2" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>1366</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" s="2" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="B623" s="2" t="s">
         <v>1170</v>
@@ -9986,7 +9991,7 @@
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="2" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B624" s="2" t="s">
         <v>1171</v>
@@ -9994,7 +9999,7 @@
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" s="2" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="B625" s="2" t="s">
         <v>1172</v>
@@ -10002,7 +10007,7 @@
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" s="2" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="B626" s="2" t="s">
         <v>1173</v>
@@ -10010,7 +10015,7 @@
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A627" s="2" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="B627" s="2" t="s">
         <v>1174</v>
@@ -10018,7 +10023,7 @@
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A628" s="2" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="B628" s="2" t="s">
         <v>1175</v>
@@ -10026,7 +10031,7 @@
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A629" s="2" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="B629" s="2" t="s">
         <v>1176</v>
@@ -10034,7 +10039,7 @@
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A630" s="2" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="B630" s="2" t="s">
         <v>1177</v>
@@ -10042,33 +10047,33 @@
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A631" s="2" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="B631" s="2" t="s">
-        <v>1336</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A632" s="2" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="C632" s="4"/>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A633" s="2" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="B633" s="2" t="s">
-        <v>1316</v>
+        <v>1445</v>
       </c>
       <c r="C633" s="4"/>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A634" s="2" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="B634" s="2" t="s">
         <v>1178</v>
@@ -10076,7 +10081,7 @@
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A635" s="2" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="B635" s="2" t="s">
         <v>1179</v>
@@ -10084,7 +10089,7 @@
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A636" s="2" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="B636" s="2" t="s">
         <v>1180</v>
@@ -10092,15 +10097,15 @@
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A637" s="2" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="B637" s="2" t="s">
-        <v>1327</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A638" s="2" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="B638" s="2" t="s">
         <v>1181</v>
@@ -10108,7 +10113,7 @@
     </row>
     <row r="639" spans="1:3" ht="35" x14ac:dyDescent="0.3">
       <c r="A639" s="2" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="B639" s="2" t="s">
         <v>1182</v>
@@ -10116,7 +10121,7 @@
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A640" s="2" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="B640" s="2" t="s">
         <v>1183</v>
@@ -10124,7 +10129,7 @@
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" s="2" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="B641" s="2" t="s">
         <v>1184</v>
@@ -10132,7 +10137,7 @@
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" s="2" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="B642" s="2" t="s">
         <v>1185</v>
@@ -10140,7 +10145,7 @@
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" s="2" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="B643" s="2" t="s">
         <v>1186</v>
@@ -10148,665 +10153,665 @@
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" s="2" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>1187</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" s="2" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="B645" s="2" t="s">
-        <v>1188</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" s="2" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" s="2" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="B647" s="2" t="s">
-        <v>1383</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" s="2" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" s="2" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="B649" s="2" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" s="2" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" s="2" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="B651" s="2" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" s="2" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" s="2" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="B653" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" s="2" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="2" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="B655" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" s="2" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A657" s="2" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="B657" s="2" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A658" s="2" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A659" s="2" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A660" s="2" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="661" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A661" s="2" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="C661" s="4"/>
       <c r="D661" s="4"/>
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A662" s="2" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="663" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A663" s="2" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A664" s="2" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="665" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A665" s="2" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="B665" s="2" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A666" s="2" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A667" s="2" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="B667" s="2" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A668" s="2" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>1338</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A669" s="2" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="670" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A670" s="2" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="671" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A671" s="2" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="672" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A672" s="2" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="673" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A673" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="674" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A674" s="2" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675" s="2" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676" s="2" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677" s="2" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678" s="2" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679" s="2" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" s="2" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681" s="2" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682" s="2" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683" s="2" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684" s="2" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685" s="2" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686" s="2" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687" s="2" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>1227</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688" s="2" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689" s="2" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690" s="2" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691" s="2" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692" s="2" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693" s="2" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>1233</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694" s="2" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="695" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A695" s="2" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" s="2" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A697" s="2" t="s">
-        <v>1317</v>
+        <v>1312</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>1318</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A698" s="2" t="s">
-        <v>1319</v>
+        <v>1314</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A699" s="2" t="s">
-        <v>1321</v>
+        <v>1316</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>1322</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A700" s="2" t="s">
-        <v>1323</v>
+        <v>1318</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>1324</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A701" s="2" t="s">
-        <v>1325</v>
+        <v>1320</v>
       </c>
       <c r="B701" s="2" t="s">
-        <v>1326</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A702" s="2" t="s">
-        <v>1328</v>
+        <v>1323</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>1345</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703" s="2" t="s">
-        <v>1329</v>
+        <v>1324</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>1330</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704" s="2" t="s">
-        <v>1331</v>
+        <v>1326</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>1337</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705" s="2" t="s">
-        <v>1332</v>
+        <v>1327</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>1333</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A706" s="2" t="s">
-        <v>1334</v>
+        <v>1329</v>
       </c>
       <c r="B706" s="2" t="s">
-        <v>1335</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A707" s="2" t="s">
-        <v>1339</v>
+        <v>1332</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>1340</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708" s="2" t="s">
-        <v>1341</v>
+        <v>1333</v>
       </c>
       <c r="B708" s="2" t="s">
-        <v>1342</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="709" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A709" s="2" t="s">
-        <v>1343</v>
+        <v>1335</v>
       </c>
       <c r="B709" s="2" t="s">
-        <v>1344</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A710" s="2" t="s">
-        <v>1346</v>
+        <v>1338</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>1353</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A711" s="2" t="s">
-        <v>1352</v>
+        <v>1344</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>1347</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A712" s="2" t="s">
-        <v>1351</v>
+        <v>1343</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>1348</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A713" s="2" t="s">
-        <v>1350</v>
+        <v>1342</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>1349</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A714" s="2" t="s">
-        <v>1354</v>
+        <v>1346</v>
       </c>
       <c r="B714" s="2" t="s">
-        <v>1355</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A715" s="2" t="s">
-        <v>1356</v>
+        <v>1348</v>
       </c>
       <c r="B715" s="2" t="s">
-        <v>1357</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A716" s="2" t="s">
-        <v>1358</v>
+        <v>1350</v>
       </c>
       <c r="B716" s="2" t="s">
-        <v>1359</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A717" s="2" t="s">
-        <v>1363</v>
+        <v>1355</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>1360</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A718" s="2" t="s">
-        <v>1362</v>
+        <v>1354</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>1361</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A719" s="2" t="s">
-        <v>1364</v>
+        <v>1356</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>1365</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A720" s="2" t="s">
-        <v>1367</v>
+        <v>1359</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>1368</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A721" s="2" t="s">
-        <v>1369</v>
+        <v>1361</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>1370</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A722" s="2" t="s">
-        <v>1384</v>
+        <v>1376</v>
       </c>
       <c r="B722" s="2" t="s">
-        <v>1385</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="723" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A723" s="2" t="s">
-        <v>1387</v>
+        <v>1379</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>1386</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="724" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A724" s="2" t="s">
-        <v>1388</v>
+        <v>1380</v>
       </c>
       <c r="B724" s="2" t="s">
-        <v>1389</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A725" s="2" t="s">
-        <v>1390</v>
+        <v>1382</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>1391</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>1396</v>
+        <v>1388</v>
       </c>
       <c r="B726" s="2" t="s">
         <v>165</v>
@@ -10814,7 +10819,7 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A727" s="2" t="s">
-        <v>1395</v>
+        <v>1387</v>
       </c>
       <c r="B727" s="2" t="s">
         <v>561</v>
@@ -10822,7 +10827,7 @@
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A728" s="2" t="s">
-        <v>1394</v>
+        <v>1386</v>
       </c>
       <c r="B728" s="2" t="s">
         <v>573</v>
@@ -10830,223 +10835,223 @@
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A729" s="2" t="s">
-        <v>1393</v>
+        <v>1385</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>1392</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A730" s="2" t="s">
-        <v>1397</v>
+        <v>1389</v>
       </c>
       <c r="B730" s="2" t="s">
-        <v>1398</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A731" s="2" t="s">
-        <v>1399</v>
+        <v>1391</v>
       </c>
       <c r="B731" s="2" t="s">
-        <v>1400</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A732" s="2" t="s">
-        <v>1401</v>
+        <v>1393</v>
       </c>
       <c r="B732" s="2" t="s">
-        <v>1402</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A733" s="2" t="s">
-        <v>1403</v>
+        <v>1395</v>
       </c>
       <c r="B733" s="2" t="s">
-        <v>1404</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A734" s="2" t="s">
-        <v>1405</v>
+        <v>1397</v>
       </c>
       <c r="B734" s="2" t="s">
-        <v>1406</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A735" s="2" t="s">
-        <v>1407</v>
+        <v>1399</v>
       </c>
       <c r="B735" s="2" t="s">
-        <v>1408</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A736" s="2" t="s">
-        <v>1409</v>
+        <v>1401</v>
       </c>
       <c r="B736" s="2" t="s">
-        <v>1410</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A737" s="2" t="s">
-        <v>1411</v>
+        <v>1403</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>1412</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A738" s="2" t="s">
-        <v>1439</v>
+        <v>1431</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>1440</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A739" s="2" t="s">
-        <v>1413</v>
+        <v>1405</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>1414</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A740" s="2" t="s">
-        <v>1415</v>
+        <v>1407</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>1416</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A741" s="2" t="s">
-        <v>1417</v>
+        <v>1409</v>
       </c>
       <c r="B741" s="2" t="s">
-        <v>1418</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A742" s="2" t="s">
-        <v>1419</v>
+        <v>1411</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>1422</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="743" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A743" s="2" t="s">
-        <v>1420</v>
+        <v>1412</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>1421</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A744" s="2" t="s">
-        <v>1423</v>
+        <v>1415</v>
       </c>
       <c r="B744" s="2" t="s">
-        <v>1424</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A745" s="2" t="s">
-        <v>1434</v>
+        <v>1426</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>1425</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A746" s="2" t="s">
-        <v>1433</v>
+        <v>1425</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>1427</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A747" s="2" t="s">
-        <v>1432</v>
+        <v>1424</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>1426</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748" s="2" t="s">
-        <v>1431</v>
+        <v>1423</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>1428</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A749" s="2" t="s">
-        <v>1430</v>
+        <v>1422</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>1429</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A750" s="2" t="s">
-        <v>1437</v>
+        <v>1429</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>1435</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A751" s="2" t="s">
-        <v>1438</v>
+        <v>1430</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1436</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A752" s="2" t="s">
-        <v>1441</v>
+        <v>1433</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>1442</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A753" s="2" t="s">
-        <v>1443</v>
+        <v>1435</v>
       </c>
       <c r="B753" s="2" t="s">
-        <v>1444</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A754" s="2" t="s">
-        <v>1445</v>
+        <v>1437</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>1446</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A755" s="2" t="s">
-        <v>1447</v>
+        <v>1439</v>
       </c>
       <c r="B755" s="2" t="s">
-        <v>1448</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A756" s="2" t="s">
-        <v>1449</v>
+        <v>1441</v>
       </c>
       <c r="B756" s="2" t="s">
         <v>1450</v>
@@ -11054,10 +11059,10 @@
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A757" s="2" t="s">
-        <v>1451</v>
+        <v>1442</v>
       </c>
       <c r="B757" s="2" t="s">
-        <v>1452</v>
+        <v>1443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add zoom factor display
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51401869-51BE-4AC5-8F58-BA515A20CB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C3248-5D5D-4047-B963-C46D25CC1337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9490" yWindow="3120" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="1465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="1467">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -2018,9 +2018,6 @@
     <t>FlatToGroundModeEnabled</t>
   </si>
   <si>
-    <t>平面显示：开</t>
-  </si>
-  <si>
     <t>AutocreateShoresMessage</t>
   </si>
   <si>
@@ -4673,6 +4670,17 @@
   </si>
   <si>
     <t>根据系统设置或手动指定，自动切换暗色模式</t>
+  </si>
+  <si>
+    <t>平面显示: 开</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScaledFactorText</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩放: %.02fx，按鼠标中键恢复</t>
   </si>
 </sst>
 </file>
@@ -5054,10 +5062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D763"/>
+  <dimension ref="A1:D764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A748" workbookViewId="0">
-      <selection activeCell="B758" sqref="B758"/>
+    <sheetView tabSelected="1" topLeftCell="A752" workbookViewId="0">
+      <selection activeCell="B760" sqref="B760"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -5068,10 +5076,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1028</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" thickTop="1" x14ac:dyDescent="0.3">
@@ -6128,7 +6136,7 @@
         <v>242</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
@@ -6808,7 +6816,7 @@
         <v>411</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -7016,7 +7024,7 @@
         <v>462</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -7296,7 +7304,7 @@
         <v>531</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -7376,7 +7384,7 @@
         <v>547</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
@@ -7536,7 +7544,7 @@
         <v>579</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -7616,7 +7624,7 @@
         <v>598</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -7624,7 +7632,7 @@
         <v>599</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -7632,7 +7640,7 @@
         <v>600</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -7640,7 +7648,7 @@
         <v>601</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -7648,7 +7656,7 @@
         <v>602</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -7656,7 +7664,7 @@
         <v>603</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -7840,7 +7848,7 @@
         <v>644</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -7904,20 +7912,20 @@
         <v>658</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>659</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="70" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B358" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="B358" s="1" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>360</v>
@@ -7925,863 +7933,863 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B360" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="B360" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B361" s="1" t="s">
         <v>665</v>
-      </c>
-      <c r="B361" s="1" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="B362" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="B362" s="1" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B363" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="B363" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B364" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="B364" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B365" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="B365" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B366" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="B366" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B367" s="1" t="s">
         <v>677</v>
-      </c>
-      <c r="B367" s="1" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B368" s="1" t="s">
         <v>679</v>
-      </c>
-      <c r="B368" s="1" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B369" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="B369" s="1" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B370" s="1" t="s">
         <v>683</v>
-      </c>
-      <c r="B370" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B371" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="B371" s="1" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B372" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="B372" s="1" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B373" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="B373" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="B374" s="1" t="s">
         <v>691</v>
-      </c>
-      <c r="B374" s="1" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B375" s="1" t="s">
         <v>693</v>
-      </c>
-      <c r="B375" s="1" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B376" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="B376" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B377" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="B377" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B378" s="1" t="s">
         <v>699</v>
-      </c>
-      <c r="B378" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B379" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="B379" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B380" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="B380" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B381" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="B381" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B382" s="1" t="s">
         <v>707</v>
-      </c>
-      <c r="B382" s="1" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B383" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="B383" s="1" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B384" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="B384" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B385" s="1" t="s">
         <v>713</v>
-      </c>
-      <c r="B385" s="1" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="B386" s="1" t="s">
         <v>715</v>
-      </c>
-      <c r="B386" s="1" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B387" s="1" t="s">
         <v>717</v>
-      </c>
-      <c r="B387" s="1" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B388" s="1" t="s">
         <v>719</v>
-      </c>
-      <c r="B388" s="1" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B389" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="B389" s="1" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B390" s="1" t="s">
         <v>723</v>
-      </c>
-      <c r="B390" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B391" s="1" t="s">
         <v>725</v>
-      </c>
-      <c r="B391" s="1" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B392" s="1" t="s">
         <v>727</v>
-      </c>
-      <c r="B392" s="1" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B397" s="1" t="s">
         <v>733</v>
-      </c>
-      <c r="B397" s="1" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B398" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="B398" s="1" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B399" s="1" t="s">
         <v>737</v>
-      </c>
-      <c r="B399" s="1" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B404" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="B404" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B405" s="1" t="s">
         <v>745</v>
-      </c>
-      <c r="B405" s="1" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B406" s="1" t="s">
         <v>747</v>
-      </c>
-      <c r="B406" s="1" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B408" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="B408" s="1" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B409" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="B409" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B410" s="1" t="s">
         <v>754</v>
-      </c>
-      <c r="B410" s="1" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B411" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="B411" s="1" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B412" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="B412" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="B413" s="1" t="s">
         <v>760</v>
-      </c>
-      <c r="B413" s="1" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B414" s="1" t="s">
         <v>762</v>
-      </c>
-      <c r="B414" s="1" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B415" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="B415" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B417" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="B417" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B418" s="1" t="s">
         <v>769</v>
-      </c>
-      <c r="B418" s="1" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B419" s="1" t="s">
         <v>771</v>
-      </c>
-      <c r="B419" s="1" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B420" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="B420" s="1" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B421" s="1" t="s">
         <v>775</v>
-      </c>
-      <c r="B421" s="1" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B422" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="B422" s="1" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B424" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="B424" s="1" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A425" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B425" s="1" t="s">
         <v>782</v>
-      </c>
-      <c r="B425" s="1" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B426" s="1" t="s">
         <v>784</v>
-      </c>
-      <c r="B426" s="1" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B427" s="1" t="s">
         <v>786</v>
-      </c>
-      <c r="B427" s="1" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B428" s="1" t="s">
         <v>788</v>
-      </c>
-      <c r="B428" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B429" s="1" t="s">
         <v>790</v>
-      </c>
-      <c r="B429" s="1" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B430" s="1" t="s">
         <v>792</v>
-      </c>
-      <c r="B430" s="1" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="B431" s="1" t="s">
         <v>794</v>
-      </c>
-      <c r="B431" s="1" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B432" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="B432" s="1" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B433" s="1" t="s">
         <v>798</v>
-      </c>
-      <c r="B433" s="1" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B434" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="B434" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B435" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="B435" s="1" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B436" s="1" t="s">
         <v>804</v>
-      </c>
-      <c r="B436" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B437" s="1" t="s">
         <v>806</v>
-      </c>
-      <c r="B437" s="1" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="B438" s="1" t="s">
         <v>808</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B439" s="1" t="s">
         <v>810</v>
-      </c>
-      <c r="B439" s="1" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B440" s="1" t="s">
         <v>812</v>
-      </c>
-      <c r="B440" s="1" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B441" s="1" t="s">
         <v>814</v>
-      </c>
-      <c r="B441" s="1" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B442" s="1" t="s">
         <v>816</v>
-      </c>
-      <c r="B442" s="1" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B443" s="1" t="s">
         <v>818</v>
-      </c>
-      <c r="B443" s="1" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B444" s="1" t="s">
         <v>820</v>
-      </c>
-      <c r="B444" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B445" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="B445" s="1" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B446" s="1" t="s">
         <v>824</v>
-      </c>
-      <c r="B446" s="1" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B447" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="B447" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B448" s="1" t="s">
         <v>828</v>
-      </c>
-      <c r="B448" s="1" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B449" s="1" t="s">
         <v>830</v>
-      </c>
-      <c r="B449" s="1" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B450" s="1" t="s">
         <v>832</v>
-      </c>
-      <c r="B450" s="1" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B451" s="1" t="s">
         <v>834</v>
-      </c>
-      <c r="B451" s="1" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="B452" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="B452" s="1" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="B453" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="B453" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="B454" s="1" t="s">
         <v>840</v>
-      </c>
-      <c r="B454" s="1" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="B455" s="1" t="s">
         <v>842</v>
-      </c>
-      <c r="B455" s="1" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B456" s="1" t="s">
         <v>844</v>
-      </c>
-      <c r="B456" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="B457" s="1" t="s">
         <v>846</v>
-      </c>
-      <c r="B457" s="1" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B458" s="1" t="s">
         <v>848</v>
-      </c>
-      <c r="B458" s="1" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B459" s="1" t="s">
         <v>850</v>
-      </c>
-      <c r="B459" s="1" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B460" s="1" t="s">
         <v>852</v>
-      </c>
-      <c r="B460" s="1" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="B461" s="1" t="s">
         <v>854</v>
-      </c>
-      <c r="B461" s="1" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B462" s="1" t="s">
         <v>856</v>
-      </c>
-      <c r="B462" s="1" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B463" s="1" t="s">
         <v>858</v>
-      </c>
-      <c r="B463" s="1" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="B464" s="1" t="s">
         <v>860</v>
-      </c>
-      <c r="B464" s="1" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="B465" s="1" t="s">
         <v>862</v>
-      </c>
-      <c r="B465" s="1" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B466" s="1" t="s">
         <v>864</v>
-      </c>
-      <c r="B466" s="1" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A467" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B467" s="1" t="s">
         <v>555</v>
@@ -8789,31 +8797,31 @@
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A468" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B468" s="1" t="s">
         <v>867</v>
-      </c>
-      <c r="B468" s="1" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A469" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="B469" s="1" t="s">
         <v>869</v>
-      </c>
-      <c r="B469" s="1" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A470" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B470" s="1" t="s">
         <v>871</v>
-      </c>
-      <c r="B470" s="1" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A471" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B471" s="1" t="s">
         <v>165</v>
@@ -8821,127 +8829,127 @@
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="B472" s="1" t="s">
         <v>874</v>
-      </c>
-      <c r="B472" s="1" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="B473" s="1" t="s">
         <v>876</v>
-      </c>
-      <c r="B473" s="1" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B474" s="1" t="s">
         <v>878</v>
-      </c>
-      <c r="B474" s="1" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A475" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B475" s="1" t="s">
         <v>880</v>
-      </c>
-      <c r="B475" s="1" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A476" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B476" s="1" t="s">
         <v>882</v>
-      </c>
-      <c r="B476" s="1" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A477" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B477" s="1" t="s">
         <v>884</v>
-      </c>
-      <c r="B477" s="1" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A478" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B478" s="1" t="s">
         <v>886</v>
-      </c>
-      <c r="B478" s="1" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A479" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B479" s="1" t="s">
         <v>888</v>
-      </c>
-      <c r="B479" s="1" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A480" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="B480" s="1" t="s">
         <v>890</v>
-      </c>
-      <c r="B480" s="1" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A481" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="B481" s="1" t="s">
         <v>892</v>
-      </c>
-      <c r="B481" s="1" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A482" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B482" s="1" t="s">
         <v>894</v>
-      </c>
-      <c r="B482" s="1" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A483" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B483" s="1" t="s">
         <v>896</v>
-      </c>
-      <c r="B483" s="1" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A484" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="B484" s="1" t="s">
         <v>898</v>
-      </c>
-      <c r="B484" s="1" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A485" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="B485" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="B485" s="1" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A486" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B486" s="1" t="s">
         <v>902</v>
-      </c>
-      <c r="B486" s="1" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A487" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B487" s="1" t="s">
         <v>364</v>
@@ -8949,15 +8957,15 @@
     </row>
     <row r="488" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A488" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B488" s="1" t="s">
         <v>905</v>
-      </c>
-      <c r="B488" s="1" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A489" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B489" s="1" t="s">
         <v>362</v>
@@ -8965,487 +8973,487 @@
     </row>
     <row r="490" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A490" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="B490" s="1" t="s">
         <v>908</v>
-      </c>
-      <c r="B490" s="1" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A491" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B491" s="1" t="s">
         <v>910</v>
-      </c>
-      <c r="B491" s="1" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A492" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B492" s="1" t="s">
         <v>912</v>
-      </c>
-      <c r="B492" s="1" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A493" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B493" s="1" t="s">
         <v>914</v>
-      </c>
-      <c r="B493" s="1" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A494" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="B494" s="1" t="s">
         <v>916</v>
-      </c>
-      <c r="B494" s="1" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A495" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B495" s="1" t="s">
         <v>918</v>
-      </c>
-      <c r="B495" s="1" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A496" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B496" s="1" t="s">
         <v>920</v>
-      </c>
-      <c r="B496" s="1" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A497" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B497" s="1" t="s">
         <v>922</v>
-      </c>
-      <c r="B497" s="1" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A498" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B498" s="1" t="s">
         <v>924</v>
-      </c>
-      <c r="B498" s="1" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A499" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B499" s="1" t="s">
         <v>926</v>
-      </c>
-      <c r="B499" s="1" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A500" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B500" s="1" t="s">
         <v>928</v>
-      </c>
-      <c r="B500" s="1" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A501" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B501" s="1" t="s">
         <v>930</v>
-      </c>
-      <c r="B501" s="1" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A502" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="B502" s="1" t="s">
         <v>932</v>
-      </c>
-      <c r="B502" s="1" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A503" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="B503" s="1" t="s">
         <v>934</v>
-      </c>
-      <c r="B503" s="1" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A504" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B504" s="1" t="s">
         <v>936</v>
-      </c>
-      <c r="B504" s="1" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A505" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="B505" s="1" t="s">
         <v>938</v>
-      </c>
-      <c r="B505" s="1" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A506" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B506" s="1" t="s">
         <v>940</v>
-      </c>
-      <c r="B506" s="1" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A507" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="B507" s="1" t="s">
         <v>942</v>
-      </c>
-      <c r="B507" s="1" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A508" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="B508" s="1" t="s">
         <v>944</v>
-      </c>
-      <c r="B508" s="1" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A509" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="B509" s="1" t="s">
         <v>946</v>
-      </c>
-      <c r="B509" s="1" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A510" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B510" s="1" t="s">
         <v>948</v>
-      </c>
-      <c r="B510" s="1" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A511" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="B511" s="1" t="s">
         <v>950</v>
-      </c>
-      <c r="B511" s="1" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A512" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="B512" s="1" t="s">
         <v>952</v>
-      </c>
-      <c r="B512" s="1" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A513" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B513" s="1" t="s">
         <v>954</v>
-      </c>
-      <c r="B513" s="1" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A514" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="B514" s="1" t="s">
         <v>956</v>
-      </c>
-      <c r="B514" s="1" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A515" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="B515" s="1" t="s">
         <v>958</v>
-      </c>
-      <c r="B515" s="1" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A516" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="B516" s="1" t="s">
         <v>960</v>
-      </c>
-      <c r="B516" s="1" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A517" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B517" s="1" t="s">
         <v>962</v>
-      </c>
-      <c r="B517" s="1" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A518" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="B518" s="1" t="s">
         <v>964</v>
-      </c>
-      <c r="B518" s="1" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A519" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="B519" s="1" t="s">
         <v>966</v>
-      </c>
-      <c r="B519" s="1" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A520" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="B520" s="1" t="s">
         <v>968</v>
-      </c>
-      <c r="B520" s="1" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A521" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B521" s="1" t="s">
         <v>970</v>
-      </c>
-      <c r="B521" s="1" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A522" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="B522" s="1" t="s">
         <v>972</v>
-      </c>
-      <c r="B522" s="1" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A523" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="B523" s="1" t="s">
         <v>974</v>
-      </c>
-      <c r="B523" s="1" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A524" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="B524" s="1" t="s">
         <v>976</v>
-      </c>
-      <c r="B524" s="1" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A525" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="B525" s="1" t="s">
         <v>978</v>
-      </c>
-      <c r="B525" s="1" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A526" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="B526" s="1" t="s">
         <v>980</v>
-      </c>
-      <c r="B526" s="1" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A527" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="B527" s="1" t="s">
         <v>982</v>
-      </c>
-      <c r="B527" s="1" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A528" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B528" s="1" t="s">
         <v>984</v>
-      </c>
-      <c r="B528" s="1" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A529" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="B529" s="1" t="s">
         <v>986</v>
-      </c>
-      <c r="B529" s="1" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A530" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="B530" s="1" t="s">
         <v>988</v>
-      </c>
-      <c r="B530" s="1" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A531" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="B531" s="1" t="s">
         <v>990</v>
-      </c>
-      <c r="B531" s="1" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A532" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="B532" s="1" t="s">
         <v>992</v>
-      </c>
-      <c r="B532" s="1" t="s">
-        <v>993</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A533" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="B533" s="1" t="s">
         <v>994</v>
-      </c>
-      <c r="B533" s="1" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A534" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="B534" s="1" t="s">
         <v>996</v>
-      </c>
-      <c r="B534" s="1" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A535" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="B535" s="1" t="s">
         <v>998</v>
-      </c>
-      <c r="B535" s="1" t="s">
-        <v>999</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A536" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="B536" s="1" t="s">
         <v>1000</v>
-      </c>
-      <c r="B536" s="1" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A537" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A538" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B538" s="1" t="s">
         <v>1003</v>
-      </c>
-      <c r="B538" s="1" t="s">
-        <v>1004</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A539" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B539" s="1" t="s">
         <v>1005</v>
-      </c>
-      <c r="B539" s="1" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A540" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B540" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="B540" s="1" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A541" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B541" s="1" t="s">
         <v>1009</v>
-      </c>
-      <c r="B541" s="1" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A542" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B542" s="1" t="s">
         <v>1011</v>
-      </c>
-      <c r="B542" s="1" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A543" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B543" s="1" t="s">
         <v>1013</v>
-      </c>
-      <c r="B543" s="1" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A544" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B544" s="1" t="s">
         <v>1015</v>
-      </c>
-      <c r="B544" s="1" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A545" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B545" s="1" t="s">
         <v>1017</v>
-      </c>
-      <c r="B545" s="1" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A546" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B546" s="1" t="s">
         <v>1019</v>
-      </c>
-      <c r="B546" s="1" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A547" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B547" s="1" t="s">
         <v>1021</v>
-      </c>
-      <c r="B547" s="1" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A548" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B548" s="1" t="s">
         <v>1023</v>
-      </c>
-      <c r="B548" s="1" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A549" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B549" s="1" t="s">
         <v>1025</v>
-      </c>
-      <c r="B549" s="1" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A550" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B550" s="1" t="s">
         <v>49</v>
@@ -9453,492 +9461,492 @@
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A551" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B551" s="2" t="s">
         <v>1030</v>
-      </c>
-      <c r="B551" s="2" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A552" s="2" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A553" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B553" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A554" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B554" s="2" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A555" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B555" s="2" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A556" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A557" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B557" s="2" t="s">
         <v>1040</v>
-      </c>
-      <c r="B557" s="2" t="s">
-        <v>1041</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A558" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B558" s="2" t="s">
         <v>1042</v>
-      </c>
-      <c r="B558" s="2" t="s">
-        <v>1043</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A559" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B559" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A560" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B560" s="2" t="s">
         <v>1045</v>
-      </c>
-      <c r="B560" s="2" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A561" s="2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B561" s="2" t="s">
         <v>1048</v>
-      </c>
-      <c r="B561" s="2" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A562" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B562" s="2" t="s">
         <v>1052</v>
-      </c>
-      <c r="B562" s="2" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
       <c r="A563" s="2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B563" s="2" t="s">
         <v>1054</v>
-      </c>
-      <c r="B563" s="2" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A564" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B564" s="2" t="s">
         <v>1057</v>
-      </c>
-      <c r="B564" s="2" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A565" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B565" s="2" t="s">
         <v>1059</v>
-      </c>
-      <c r="B565" s="2" t="s">
-        <v>1060</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A566" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B566" s="2" t="s">
         <v>1062</v>
-      </c>
-      <c r="B566" s="2" t="s">
-        <v>1063</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A567" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B567" s="2" t="s">
         <v>1064</v>
-      </c>
-      <c r="B567" s="2" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A568" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B568" s="2" t="s">
         <v>1066</v>
-      </c>
-      <c r="B568" s="2" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A569" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B569" s="2" t="s">
         <v>1069</v>
-      </c>
-      <c r="B569" s="2" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A570" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B570" s="2" t="s">
         <v>1071</v>
-      </c>
-      <c r="B570" s="2" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A571" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B571" s="2" t="s">
         <v>1075</v>
-      </c>
-      <c r="B571" s="2" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A572" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B572" s="2" t="s">
         <v>1073</v>
-      </c>
-      <c r="B572" s="2" t="s">
-        <v>1074</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A573" s="2" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B573" s="2" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A574" s="2" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B574" s="2" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A575" s="2" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B575" s="2" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A576" s="2" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B576" s="2" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A577" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B577" s="2" t="s">
         <v>1087</v>
-      </c>
-      <c r="B577" s="2" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A578" s="2" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B578" s="2" t="s">
         <v>1091</v>
-      </c>
-      <c r="B578" s="2" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A579" s="2" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B579" s="2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A580" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B580" s="2" t="s">
         <v>1089</v>
-      </c>
-      <c r="B580" s="2" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A581" s="2" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B581" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A582" s="2" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A583" s="2" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B583" s="2" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A584" s="2" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A585" s="2" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B585" s="2" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A586" s="2" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A587" s="2" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B587" s="2" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A588" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B588" s="2" t="s">
         <v>1107</v>
-      </c>
-      <c r="B588" s="2" t="s">
-        <v>1108</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A589" s="2" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B589" s="2" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A590" s="2" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B590" s="2" t="s">
         <v>1111</v>
-      </c>
-      <c r="B590" s="2" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A591" s="2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B591" s="2" t="s">
         <v>1113</v>
-      </c>
-      <c r="B591" s="2" t="s">
-        <v>1114</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A592" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B592" s="2" t="s">
         <v>1115</v>
-      </c>
-      <c r="B592" s="2" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A593" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B593" s="2" t="s">
         <v>1117</v>
-      </c>
-      <c r="B593" s="2" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A594" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B594" s="2" t="s">
         <v>1119</v>
-      </c>
-      <c r="B594" s="2" t="s">
-        <v>1120</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A595" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B595" s="2" t="s">
         <v>1121</v>
-      </c>
-      <c r="B595" s="2" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A596" s="2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B596" s="2" t="s">
         <v>1123</v>
-      </c>
-      <c r="B596" s="2" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A597" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B597" s="2" t="s">
         <v>1125</v>
-      </c>
-      <c r="B597" s="2" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B598" s="2" t="s">
         <v>1127</v>
-      </c>
-      <c r="B598" s="2" t="s">
-        <v>1128</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A599" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B599" s="2" t="s">
         <v>1129</v>
-      </c>
-      <c r="B599" s="2" t="s">
-        <v>1130</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B600" s="2" t="s">
         <v>1131</v>
-      </c>
-      <c r="B600" s="2" t="s">
-        <v>1132</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A601" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B601" s="2" t="s">
         <v>1133</v>
-      </c>
-      <c r="B601" s="2" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602" s="2" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B602" s="2" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603" s="2" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B603" s="2" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A604" s="2" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B604" s="2" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B605" s="2" t="s">
         <v>1141</v>
-      </c>
-      <c r="B605" s="2" t="s">
-        <v>1142</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A606" s="2" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B606" s="2" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="607" spans="1:2" ht="70" x14ac:dyDescent="0.3">
       <c r="A607" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B607" s="2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A608" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B608" s="2" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A609" s="2" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B609" s="2" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A610" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A611" s="2" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B611" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A612" s="2" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B612" s="2" t="s">
         <v>67</v>
@@ -9946,915 +9954,915 @@
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A613" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B613" s="2" t="s">
         <v>1154</v>
-      </c>
-      <c r="B613" s="2" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A614" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B614" s="2" t="s">
         <v>1156</v>
-      </c>
-      <c r="B614" s="2" t="s">
-        <v>1157</v>
       </c>
     </row>
     <row r="615" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A615" s="2" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B615" s="2" t="s">
         <v>1158</v>
-      </c>
-      <c r="B615" s="2" t="s">
-        <v>1159</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A616" s="2" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B616" s="2" t="s">
         <v>1160</v>
-      </c>
-      <c r="B616" s="2" t="s">
-        <v>1161</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A617" s="2" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="B617" s="2" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A618" s="2" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B618" s="2" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A619" s="2" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B619" s="2" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="620" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A620" s="2" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B620" s="2" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" s="2" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B621" s="2" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="2" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" s="2" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B623" s="2" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="2" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" s="2" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B625" s="2" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A627" s="2" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B627" s="2" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A628" s="2" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A629" s="2" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B629" s="2" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A630" s="2" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B630" s="2" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A631" s="2" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B631" s="2" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A632" s="2" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C632" s="4"/>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A633" s="2" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B633" s="2" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="C633" s="4"/>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A634" s="2" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B634" s="2" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A635" s="2" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B635" s="2" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A636" s="2" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B636" s="2" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A637" s="2" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B637" s="2" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A638" s="2" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B638" s="2" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="639" spans="1:3" ht="35" x14ac:dyDescent="0.3">
       <c r="A639" s="2" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B639" s="2" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A640" s="2" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" s="2" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B641" s="2" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" s="2" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" s="2" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" s="2" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" s="2" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B645" s="2" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" s="2" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" s="2" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B647" s="2" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" s="2" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" s="2" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B649" s="2" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" s="2" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" s="2" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B651" s="2" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" s="2" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" s="2" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B653" s="2" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" s="2" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="2" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B655" s="2" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" s="2" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A657" s="2" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B657" s="2" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A658" s="2" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A659" s="2" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A660" s="2" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="661" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A661" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C661" s="4"/>
       <c r="D661" s="4"/>
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A662" s="2" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="663" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A663" s="2" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A664" s="2" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="665" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A665" s="2" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B665" s="2" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A666" s="2" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A667" s="2" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B667" s="2" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A668" s="2" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A669" s="2" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="670" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A670" s="2" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="671" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A671" s="2" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="672" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A672" s="2" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="673" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A673" s="2" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="674" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A674" s="2" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675" s="2" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676" s="2" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677" s="2" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678" s="2" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679" s="2" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" s="2" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681" s="2" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682" s="2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683" s="2" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684" s="2" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685" s="2" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686" s="2" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687" s="2" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688" s="2" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689" s="2" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690" s="2" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691" s="2" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692" s="2" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693" s="2" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="695" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A695" s="2" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A697" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B697" s="2" t="s">
         <v>1312</v>
-      </c>
-      <c r="B697" s="2" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A698" s="2" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B698" s="2" t="s">
         <v>1314</v>
-      </c>
-      <c r="B698" s="2" t="s">
-        <v>1315</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A699" s="2" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B699" s="2" t="s">
         <v>1316</v>
-      </c>
-      <c r="B699" s="2" t="s">
-        <v>1317</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A700" s="2" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B700" s="2" t="s">
         <v>1318</v>
-      </c>
-      <c r="B700" s="2" t="s">
-        <v>1319</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A701" s="2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B701" s="2" t="s">
         <v>1320</v>
-      </c>
-      <c r="B701" s="2" t="s">
-        <v>1321</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A702" s="2" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703" s="2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B703" s="2" t="s">
         <v>1324</v>
-      </c>
-      <c r="B703" s="2" t="s">
-        <v>1325</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B705" s="2" t="s">
         <v>1327</v>
-      </c>
-      <c r="B705" s="2" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A706" s="2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B706" s="2" t="s">
         <v>1329</v>
-      </c>
-      <c r="B706" s="2" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A707" s="2" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708" s="2" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B708" s="2" t="s">
         <v>1333</v>
-      </c>
-      <c r="B708" s="2" t="s">
-        <v>1334</v>
       </c>
     </row>
     <row r="709" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A709" s="2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B709" s="2" t="s">
         <v>1335</v>
-      </c>
-      <c r="B709" s="2" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A710" s="2" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A711" s="2" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A712" s="2" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A713" s="2" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A714" s="2" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B714" s="2" t="s">
         <v>1346</v>
-      </c>
-      <c r="B714" s="2" t="s">
-        <v>1347</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A715" s="2" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B715" s="2" t="s">
         <v>1348</v>
-      </c>
-      <c r="B715" s="2" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A716" s="2" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B716" s="2" t="s">
         <v>1350</v>
-      </c>
-      <c r="B716" s="2" t="s">
-        <v>1351</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A717" s="2" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A718" s="2" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A719" s="2" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B719" s="2" t="s">
         <v>1356</v>
-      </c>
-      <c r="B719" s="2" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A720" s="2" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B720" s="2" t="s">
         <v>1359</v>
-      </c>
-      <c r="B720" s="2" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A721" s="2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B721" s="2" t="s">
         <v>1361</v>
-      </c>
-      <c r="B721" s="2" t="s">
-        <v>1362</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A722" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B722" s="2" t="s">
         <v>1376</v>
-      </c>
-      <c r="B722" s="2" t="s">
-        <v>1377</v>
       </c>
     </row>
     <row r="723" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A723" s="2" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="724" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A724" s="2" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B724" s="2" t="s">
         <v>1380</v>
-      </c>
-      <c r="B724" s="2" t="s">
-        <v>1381</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A725" s="2" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B725" s="2" t="s">
         <v>1382</v>
-      </c>
-      <c r="B725" s="2" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B726" s="2" t="s">
         <v>165</v>
@@ -10862,7 +10870,7 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A727" s="2" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="B727" s="2" t="s">
         <v>561</v>
@@ -10870,7 +10878,7 @@
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A728" s="2" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B728" s="2" t="s">
         <v>573</v>
@@ -10878,282 +10886,290 @@
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A729" s="2" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A730" s="2" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B730" s="2" t="s">
         <v>1389</v>
-      </c>
-      <c r="B730" s="2" t="s">
-        <v>1390</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A731" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B731" s="2" t="s">
         <v>1391</v>
-      </c>
-      <c r="B731" s="2" t="s">
-        <v>1392</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A732" s="2" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B732" s="2" t="s">
         <v>1393</v>
-      </c>
-      <c r="B732" s="2" t="s">
-        <v>1394</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A733" s="2" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B733" s="2" t="s">
         <v>1395</v>
-      </c>
-      <c r="B733" s="2" t="s">
-        <v>1396</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A734" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B734" s="2" t="s">
         <v>1397</v>
-      </c>
-      <c r="B734" s="2" t="s">
-        <v>1398</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A735" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B735" s="2" t="s">
         <v>1399</v>
-      </c>
-      <c r="B735" s="2" t="s">
-        <v>1400</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A736" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B736" s="2" t="s">
         <v>1401</v>
-      </c>
-      <c r="B736" s="2" t="s">
-        <v>1402</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A737" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B737" s="2" t="s">
         <v>1403</v>
-      </c>
-      <c r="B737" s="2" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A738" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B738" s="2" t="s">
         <v>1431</v>
-      </c>
-      <c r="B738" s="2" t="s">
-        <v>1432</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A739" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B739" s="2" t="s">
         <v>1405</v>
-      </c>
-      <c r="B739" s="2" t="s">
-        <v>1406</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A740" s="2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B740" s="2" t="s">
         <v>1407</v>
-      </c>
-      <c r="B740" s="2" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A741" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B741" s="2" t="s">
         <v>1409</v>
-      </c>
-      <c r="B741" s="2" t="s">
-        <v>1410</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A742" s="2" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="743" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A743" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B743" s="2" t="s">
         <v>1412</v>
-      </c>
-      <c r="B743" s="2" t="s">
-        <v>1413</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A744" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B744" s="2" t="s">
         <v>1415</v>
-      </c>
-      <c r="B744" s="2" t="s">
-        <v>1416</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A745" s="2" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A746" s="2" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A747" s="2" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748" s="2" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A749" s="2" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A750" s="2" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A751" s="2" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A752" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B752" s="2" t="s">
         <v>1433</v>
-      </c>
-      <c r="B752" s="2" t="s">
-        <v>1434</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A753" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B753" s="2" t="s">
         <v>1435</v>
-      </c>
-      <c r="B753" s="2" t="s">
-        <v>1436</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A754" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B754" s="2" t="s">
         <v>1437</v>
-      </c>
-      <c r="B754" s="2" t="s">
-        <v>1438</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A755" s="2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B755" s="2" t="s">
         <v>1439</v>
-      </c>
-      <c r="B755" s="2" t="s">
-        <v>1440</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A756" s="2" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A757" s="2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B757" s="2" t="s">
         <v>1442</v>
-      </c>
-      <c r="B757" s="2" t="s">
-        <v>1443</v>
       </c>
     </row>
     <row r="758" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
       <c r="A758" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B758" s="2" t="s">
         <v>1461</v>
-      </c>
-      <c r="B758" s="2" t="s">
-        <v>1462</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A759" s="2" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A760" s="2" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A761" s="2" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A762" s="2" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A763" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B763" s="2" t="s">
         <v>1463</v>
       </c>
-      <c r="B763" s="2" t="s">
-        <v>1464</v>
+    </row>
+    <row r="764" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A764" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B764" s="2" t="s">
+        <v>1466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add trigger annotation dlg
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C3248-5D5D-4047-B963-C46D25CC1337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AA44D3-E46B-4652-A507-7EBCB412FDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9490" yWindow="3120" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="1467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="1473">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4681,6 +4681,28 @@
   </si>
   <si>
     <t>缩放: %.02fx，按鼠标中键恢复</t>
+  </si>
+  <si>
+    <t>触发注释</t>
+  </si>
+  <si>
+    <t>当前对象: %s</t>
+  </si>
+  <si>
+    <t>触发注释\tCtrl+Shift+A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.MapTools.TriggerAnnotation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerAnnotation.Text</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerAnnotation.Title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5062,10 +5084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D764"/>
+  <dimension ref="A1:D767"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A752" workbookViewId="0">
-      <selection activeCell="B760" sqref="B760"/>
+    <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
+      <selection activeCell="B761" sqref="B761"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11172,6 +11194,30 @@
         <v>1466</v>
       </c>
     </row>
+    <row r="765" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A765" s="2" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B765" s="2" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="766" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A766" s="2" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B766" s="2" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A767" s="2" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B767" s="2" t="s">
+        <v>1469</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support damage fires, add map renderer
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3752BBD-FF6E-4D85-A5DF-874BC65ABBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A134F-4E82-4CDE-9D54-F6711C59F0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9400" yWindow="5600" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="1505">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4689,40 +4689,131 @@
     <t>当前对象: %s</t>
   </si>
   <si>
+    <t>TriggerAnnotation.Text</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerAnnotation.Title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>本文件编码为 UTF8，请使用此格式打开</t>
+  </si>
+  <si>
+    <t>打开ini和地图文件时自动推断编码</t>
+  </si>
+  <si>
+    <t>总是以UTF8编码保存地图</t>
+  </si>
+  <si>
+    <t>Options.UTF8Support.AlwaysSaveAsUTF8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UTF8Support.InferEncoding</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SaveMap_FileEncodingComment1_UTF8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图注释\tAlt+9</t>
+  </si>
+  <si>
+    <t>受损火焰\tAlt+Num0</t>
+  </si>
+  <si>
+    <t>内存分配失败，无法渲染全图</t>
+  </si>
+  <si>
+    <t>Menu.Display.Annotations</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Display.DamageFires</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllocFullMapBitmapFailed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图渲染选项</t>
+  </si>
+  <si>
+    <t>渲染区域</t>
+  </si>
+  <si>
+    <t>渲染图层</t>
+  </si>
+  <si>
+    <t>可见区域</t>
+  </si>
+  <si>
+    <t>全地图</t>
+  </si>
+  <si>
+    <t>游戏内效果</t>
+  </si>
+  <si>
+    <t>当前图层</t>
+  </si>
+  <si>
+    <t>MapRendererDlgCurrentlayers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgIngame</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgFullsize</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgLocalsize</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgRenderlayers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgRenderSize</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgCaption</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>触发注释\tCtrl+Shift+A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Menu.MapTools.TriggerAnnotation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TriggerAnnotation.Text</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TriggerAnnotation.Title</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>本文件编码为 UTF8，请使用此格式打开</t>
-  </si>
-  <si>
-    <t>打开ini和地图文件时自动推断编码</t>
-  </si>
-  <si>
-    <t>总是以UTF8编码保存地图</t>
-  </si>
-  <si>
-    <t>Options.UTF8Support.AlwaysSaveAsUTF8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.UTF8Support.InferEncoding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SaveMap_FileEncodingComment1_UTF8</t>
+  </si>
+  <si>
+    <t>Menu.MapTools.MapRenderer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Edit.TriggerAnnotation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgTips</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图渲染器会使用当前光照沙盒设置</t>
+  </si>
+  <si>
+    <t>地图渲染已输出至：</t>
+  </si>
+  <si>
+    <t>MapRendererSuccess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图渲染器</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5105,10 +5196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D770"/>
+  <dimension ref="A1:D783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
-      <selection activeCell="B763" sqref="B763"/>
+    <sheetView tabSelected="1" topLeftCell="A779" workbookViewId="0">
+      <selection activeCell="B784" sqref="B784"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11217,7 +11308,7 @@
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A765" s="2" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="B765" s="2" t="s">
         <v>1467</v>
@@ -11225,7 +11316,7 @@
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A766" s="2" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="B766" s="2" t="s">
         <v>1468</v>
@@ -11233,34 +11324,138 @@
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A767" s="2" t="s">
-        <v>1470</v>
+        <v>1476</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>1469</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A768" s="2" t="s">
-        <v>1478</v>
+        <v>1475</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A769" s="2" t="s">
-        <v>1477</v>
+        <v>1474</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A770" s="2" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>1475</v>
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A771" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B771" s="2" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A772" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B772" s="2" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A773" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B773" s="2" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A774" s="2" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B774" s="2" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A775" s="2" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B775" s="2" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A776" s="2" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B776" s="2" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A777" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B777" s="2" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A778" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B778" s="2" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A779" s="2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B779" s="2" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="780" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A780" s="2" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B780" s="2" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="781" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A781" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B781" s="2" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="782" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A782" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B782" s="2" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="783" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A783" s="2" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B783" s="2" t="s">
+        <v>1502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix map renderer bugs, add progress dlg
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447E986E-9B91-4FAA-8C80-8663967CF60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB20C063-AE1C-4B0A-A701-BF3FA3DC0A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="1525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="1527">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4889,6 +4889,13 @@
   <si>
     <t>标记游戏者位置</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererProgressText</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>渲染中，请稍后...</t>
   </si>
 </sst>
 </file>
@@ -5270,10 +5277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D795"/>
+  <dimension ref="A1:D796"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A764" workbookViewId="0">
-      <selection activeCell="B793" sqref="B793"/>
+      <selection activeCell="B785" sqref="B785"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11628,6 +11635,14 @@
         <v>1513</v>
       </c>
     </row>
+    <row r="796" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A796" s="2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B796" s="2" t="s">
+        <v>1526</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support extra ore placement & random ore
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D90720B-B25E-4521-9CA7-42A55BA0B1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E41C86B-3396-43A2-9976-C3835BD0D743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9400" yWindow="5600" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="1537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="1545">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4931,6 +4931,34 @@
   </si>
   <si>
     <t>距离标尺</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>绘制矿石3</t>
+  </si>
+  <si>
+    <t>绘制矿石4</t>
+  </si>
+  <si>
+    <t>摆放矿石时随机图像</t>
+  </si>
+  <si>
+    <t>支持额外矿石类型的摆放</t>
+  </si>
+  <si>
+    <t>Options.ObjectBrowser.Ore.ExtraSupport</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ObjectBrowser.Ore.RandomPlacement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DrawTib4ObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DrawTib3ObList</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5313,10 +5341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D801"/>
+  <dimension ref="A1:D805"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A704" workbookViewId="0">
-      <selection activeCell="B710" sqref="B710"/>
+    <sheetView tabSelected="1" topLeftCell="A791" workbookViewId="0">
+      <selection activeCell="A801" sqref="A801"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11719,6 +11747,38 @@
         <v>1533</v>
       </c>
     </row>
+    <row r="802" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A802" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B802" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A803" s="2" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B803" s="2" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="804" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A804" s="2" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B804" s="2" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="805" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A805" s="2" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B805" s="2" t="s">
+        <v>1540</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add random tile placement
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E94FCC-A89E-4276-AA6E-86AEF5AF2250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC715023-B51C-4944-A9A7-6B56005A2B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9400" yWindow="5600" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="1547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="1549">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4967,6 +4967,13 @@
   </si>
   <si>
     <t>剪切\tCtrl+X</t>
+  </si>
+  <si>
+    <t>PlaceRandomTileObList</t>
+  </si>
+  <si>
+    <t>随机地形</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5348,10 +5355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D806"/>
+  <dimension ref="A1:D807"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A791" workbookViewId="0">
-      <selection activeCell="B799" sqref="B799"/>
+      <selection activeCell="B807" sqref="B807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -11794,6 +11801,14 @@
         <v>1546</v>
       </c>
     </row>
+    <row r="807" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A807" s="2" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B807" s="2" t="s">
+        <v>1548</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
map renderer supports jpg format
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC715023-B51C-4944-A9A7-6B56005A2B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20513DEA-B5DF-486E-A802-B801FBF5B070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9400" yWindow="5600" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="1549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="1553">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3489,9 +3489,6 @@
     <t>MultiSelectionOptionConnected</t>
   </si>
   <si>
-    <t>相连</t>
-  </si>
-  <si>
     <t>MultiSelectionOptionSameTileSet</t>
   </si>
   <si>
@@ -4973,6 +4970,24 @@
   </si>
   <si>
     <t>随机地形</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiSelectionOptionConnected8Ways</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8向相连</t>
+  </si>
+  <si>
+    <t>4向相连</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgFileFormat</t>
+  </si>
+  <si>
+    <t>文件格式</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5355,10 +5370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D807"/>
+  <dimension ref="A1:D809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A791" workbookViewId="0">
-      <selection activeCell="B807" sqref="B807"/>
+    <sheetView tabSelected="1" topLeftCell="A797" workbookViewId="0">
+      <selection activeCell="B809" sqref="B809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -7109,7 +7124,7 @@
         <v>411</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -7317,7 +7332,7 @@
         <v>462</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -7597,7 +7612,7 @@
         <v>531</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -7837,7 +7852,7 @@
         <v>579</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -7917,7 +7932,7 @@
         <v>598</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -7925,7 +7940,7 @@
         <v>599</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -7933,7 +7948,7 @@
         <v>600</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -7941,7 +7956,7 @@
         <v>601</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -7949,7 +7964,7 @@
         <v>602</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -7957,7 +7972,7 @@
         <v>603</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -8141,7 +8156,7 @@
         <v>644</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -8205,7 +8220,7 @@
         <v>658</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="70" x14ac:dyDescent="0.3">
@@ -8733,7 +8748,7 @@
         <v>778</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
@@ -10122,55 +10137,55 @@
         <v>1124</v>
       </c>
       <c r="B597" s="2" t="s">
-        <v>1125</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B598" s="2" t="s">
         <v>1126</v>
-      </c>
-      <c r="B598" s="2" t="s">
-        <v>1127</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A599" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B599" s="2" t="s">
         <v>1128</v>
-      </c>
-      <c r="B599" s="2" t="s">
-        <v>1129</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B600" s="2" t="s">
         <v>1130</v>
-      </c>
-      <c r="B600" s="2" t="s">
-        <v>1131</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A601" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B601" s="2" t="s">
         <v>1132</v>
-      </c>
-      <c r="B601" s="2" t="s">
-        <v>1133</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602" s="2" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B602" s="2" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603" s="2" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B603" s="2" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
@@ -10178,23 +10193,23 @@
         <v>1067</v>
       </c>
       <c r="B604" s="2" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605" s="2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B605" s="2" t="s">
         <v>1140</v>
-      </c>
-      <c r="B605" s="2" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A606" s="2" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B606" s="2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="607" spans="1:2" ht="70" x14ac:dyDescent="0.3">
@@ -10202,44 +10217,44 @@
         <v>1060</v>
       </c>
       <c r="B607" s="2" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A608" s="2" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B608" s="2" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A609" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B609" s="2" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A610" s="2" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A611" s="2" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B611" s="2" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A612" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B612" s="2" t="s">
         <v>67</v>
@@ -10247,915 +10262,915 @@
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A613" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B613" s="2" t="s">
         <v>1153</v>
-      </c>
-      <c r="B613" s="2" t="s">
-        <v>1154</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A614" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B614" s="2" t="s">
         <v>1155</v>
-      </c>
-      <c r="B614" s="2" t="s">
-        <v>1156</v>
       </c>
     </row>
     <row r="615" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A615" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B615" s="2" t="s">
         <v>1157</v>
-      </c>
-      <c r="B615" s="2" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A616" s="2" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B616" s="2" t="s">
         <v>1159</v>
-      </c>
-      <c r="B616" s="2" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A617" s="2" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B617" s="2" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A618" s="2" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="B618" s="2" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A619" s="2" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B619" s="2" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="620" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A620" s="2" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B620" s="2" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" s="2" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B621" s="2" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="2" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" s="2" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B623" s="2" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="2" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" s="2" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B625" s="2" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" s="2" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A627" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B627" s="2" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A628" s="2" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A629" s="2" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B629" s="2" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A630" s="2" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B630" s="2" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A631" s="2" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B631" s="2" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A632" s="2" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C632" s="4"/>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A633" s="2" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B633" s="2" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="C633" s="4"/>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A634" s="2" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B634" s="2" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A635" s="2" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B635" s="2" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A636" s="2" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B636" s="2" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A637" s="2" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B637" s="2" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A638" s="2" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B638" s="2" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="639" spans="1:3" ht="35" x14ac:dyDescent="0.3">
       <c r="A639" s="2" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B639" s="2" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A640" s="2" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" s="2" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B641" s="2" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" s="2" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" s="2" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" s="2" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" s="2" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B645" s="2" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" s="2" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" s="2" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B647" s="2" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" s="2" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" s="2" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B649" s="2" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" s="2" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" s="2" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B651" s="2" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" s="2" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" s="2" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B653" s="2" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" s="2" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="2" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B655" s="2" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" s="2" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A657" s="2" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B657" s="2" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A658" s="2" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A659" s="2" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A660" s="2" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="661" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A661" s="2" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C661" s="4"/>
       <c r="D661" s="4"/>
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A662" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="663" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A663" s="2" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A664" s="2" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="665" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A665" s="2" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B665" s="2" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A666" s="2" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A667" s="2" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B667" s="2" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A668" s="2" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A669" s="2" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="670" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A670" s="2" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="671" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A671" s="2" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="672" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A672" s="2" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="673" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A673" s="2" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="674" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A674" s="2" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675" s="2" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676" s="2" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677" s="2" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678" s="2" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679" s="2" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" s="2" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681" s="2" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682" s="2" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683" s="2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684" s="2" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685" s="2" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686" s="2" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687" s="2" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688" s="2" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689" s="2" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690" s="2" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691" s="2" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692" s="2" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693" s="2" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694" s="2" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="695" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A695" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" s="2" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A697" s="2" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B697" s="2" t="s">
         <v>1311</v>
-      </c>
-      <c r="B697" s="2" t="s">
-        <v>1312</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A698" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B698" s="2" t="s">
         <v>1313</v>
-      </c>
-      <c r="B698" s="2" t="s">
-        <v>1314</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A699" s="2" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B699" s="2" t="s">
         <v>1315</v>
-      </c>
-      <c r="B699" s="2" t="s">
-        <v>1316</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A700" s="2" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B700" s="2" t="s">
         <v>1317</v>
-      </c>
-      <c r="B700" s="2" t="s">
-        <v>1318</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A701" s="2" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B701" s="2" t="s">
         <v>1319</v>
-      </c>
-      <c r="B701" s="2" t="s">
-        <v>1320</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A702" s="2" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703" s="2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B703" s="2" t="s">
         <v>1323</v>
-      </c>
-      <c r="B703" s="2" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704" s="2" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705" s="2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B705" s="2" t="s">
         <v>1326</v>
-      </c>
-      <c r="B705" s="2" t="s">
-        <v>1327</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A706" s="2" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B706" s="2" t="s">
         <v>1328</v>
-      </c>
-      <c r="B706" s="2" t="s">
-        <v>1329</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A707" s="2" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708" s="2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B708" s="2" t="s">
         <v>1332</v>
-      </c>
-      <c r="B708" s="2" t="s">
-        <v>1333</v>
       </c>
     </row>
     <row r="709" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A709" s="2" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B709" s="2" t="s">
         <v>1334</v>
-      </c>
-      <c r="B709" s="2" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A710" s="2" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A711" s="2" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A712" s="2" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A713" s="2" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A714" s="2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B714" s="2" t="s">
         <v>1344</v>
-      </c>
-      <c r="B714" s="2" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A715" s="2" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B715" s="2" t="s">
         <v>1346</v>
-      </c>
-      <c r="B715" s="2" t="s">
-        <v>1347</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A716" s="2" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B716" s="2" t="s">
         <v>1348</v>
-      </c>
-      <c r="B716" s="2" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A717" s="2" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A718" s="2" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A719" s="2" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B719" s="2" t="s">
         <v>1354</v>
-      </c>
-      <c r="B719" s="2" t="s">
-        <v>1355</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A720" s="2" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B720" s="2" t="s">
         <v>1357</v>
-      </c>
-      <c r="B720" s="2" t="s">
-        <v>1358</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A721" s="2" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B721" s="2" t="s">
         <v>1359</v>
-      </c>
-      <c r="B721" s="2" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A722" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B722" s="2" t="s">
         <v>1374</v>
-      </c>
-      <c r="B722" s="2" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="723" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A723" s="2" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="724" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A724" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B724" s="2" t="s">
         <v>1378</v>
-      </c>
-      <c r="B724" s="2" t="s">
-        <v>1379</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A725" s="2" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B725" s="2" t="s">
         <v>1380</v>
-      </c>
-      <c r="B725" s="2" t="s">
-        <v>1381</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B726" s="2" t="s">
         <v>165</v>
@@ -11163,7 +11178,7 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A727" s="2" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B727" s="2" t="s">
         <v>561</v>
@@ -11171,7 +11186,7 @@
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A728" s="2" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B728" s="2" t="s">
         <v>573</v>
@@ -11179,479 +11194,479 @@
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A729" s="2" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A730" s="2" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B730" s="2" t="s">
         <v>1387</v>
-      </c>
-      <c r="B730" s="2" t="s">
-        <v>1388</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A731" s="2" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B731" s="2" t="s">
         <v>1389</v>
-      </c>
-      <c r="B731" s="2" t="s">
-        <v>1390</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A732" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B732" s="2" t="s">
         <v>1391</v>
-      </c>
-      <c r="B732" s="2" t="s">
-        <v>1392</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A733" s="2" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B733" s="2" t="s">
         <v>1393</v>
-      </c>
-      <c r="B733" s="2" t="s">
-        <v>1394</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A734" s="2" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B734" s="2" t="s">
         <v>1395</v>
-      </c>
-      <c r="B734" s="2" t="s">
-        <v>1396</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A735" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B735" s="2" t="s">
         <v>1397</v>
-      </c>
-      <c r="B735" s="2" t="s">
-        <v>1398</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A736" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B736" s="2" t="s">
         <v>1399</v>
-      </c>
-      <c r="B736" s="2" t="s">
-        <v>1400</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A737" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B737" s="2" t="s">
         <v>1401</v>
-      </c>
-      <c r="B737" s="2" t="s">
-        <v>1402</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A738" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B738" s="2" t="s">
         <v>1429</v>
-      </c>
-      <c r="B738" s="2" t="s">
-        <v>1430</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A739" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B739" s="2" t="s">
         <v>1403</v>
-      </c>
-      <c r="B739" s="2" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A740" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B740" s="2" t="s">
         <v>1405</v>
-      </c>
-      <c r="B740" s="2" t="s">
-        <v>1406</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A741" s="2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B741" s="2" t="s">
         <v>1407</v>
-      </c>
-      <c r="B741" s="2" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A742" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="743" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A743" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B743" s="2" t="s">
         <v>1410</v>
-      </c>
-      <c r="B743" s="2" t="s">
-        <v>1411</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A744" s="2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B744" s="2" t="s">
         <v>1413</v>
-      </c>
-      <c r="B744" s="2" t="s">
-        <v>1414</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A745" s="2" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A746" s="2" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A747" s="2" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748" s="2" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A749" s="2" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A750" s="2" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A751" s="2" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A752" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B752" s="2" t="s">
         <v>1431</v>
-      </c>
-      <c r="B752" s="2" t="s">
-        <v>1432</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A753" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B753" s="2" t="s">
         <v>1433</v>
-      </c>
-      <c r="B753" s="2" t="s">
-        <v>1434</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A754" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B754" s="2" t="s">
         <v>1435</v>
-      </c>
-      <c r="B754" s="2" t="s">
-        <v>1436</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A755" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B755" s="2" t="s">
         <v>1437</v>
-      </c>
-      <c r="B755" s="2" t="s">
-        <v>1438</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A756" s="2" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A757" s="2" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B757" s="2" t="s">
         <v>1440</v>
-      </c>
-      <c r="B757" s="2" t="s">
-        <v>1441</v>
       </c>
     </row>
     <row r="758" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
       <c r="A758" s="2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B758" s="2" t="s">
         <v>1459</v>
-      </c>
-      <c r="B758" s="2" t="s">
-        <v>1460</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A759" s="2" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A760" s="2" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A761" s="2" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A762" s="2" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A763" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B763" s="2" t="s">
         <v>1461</v>
-      </c>
-      <c r="B763" s="2" t="s">
-        <v>1462</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A764" s="2" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B764" s="2" t="s">
         <v>1464</v>
-      </c>
-      <c r="B764" s="2" t="s">
-        <v>1465</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A765" s="2" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A766" s="2" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B766" s="2" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A767" s="2" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A768" s="2" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A769" s="2" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A770" s="2" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A771" s="2" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A772" s="2" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A773" s="2" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A774" s="2" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A775" s="2" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A776" s="2" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A777" s="2" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A778" s="2" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A779" s="2" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A780" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A781" s="2" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A782" s="2" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A783" s="2" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A784" s="2" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A785" s="2" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B785" s="2" t="s">
         <v>1504</v>
-      </c>
-      <c r="B785" s="2" t="s">
-        <v>1505</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A786" s="2" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A787" s="2" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A788" s="2" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B788" s="2" t="s">
         <v>486</v>
@@ -11659,7 +11674,7 @@
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A789" s="2" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="B789" s="2" t="s">
         <v>488</v>
@@ -11667,7 +11682,7 @@
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A790" s="2" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B790" s="2" t="s">
         <v>490</v>
@@ -11675,7 +11690,7 @@
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A791" s="2" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="B791" s="2" t="s">
         <v>492</v>
@@ -11683,130 +11698,146 @@
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A792" s="2" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A793" s="2" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A794" s="2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A795" s="2" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A796" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B796" s="2" t="s">
         <v>1523</v>
-      </c>
-      <c r="B796" s="2" t="s">
-        <v>1524</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A797" s="2" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A798" s="2" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A799" s="2" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A800" s="2" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B800" s="2" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A801" s="2" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A802" s="2" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A803" s="2" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="804" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A804" s="2" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="805" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A805" s="2" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A806" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B806" s="2" t="s">
         <v>1545</v>
-      </c>
-      <c r="B806" s="2" t="s">
-        <v>1546</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A807" s="2" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B807" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="B807" s="2" t="s">
+    </row>
+    <row r="808" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A808" s="2" t="s">
         <v>1548</v>
+      </c>
+      <c r="B808" s="2" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="809" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A809" s="2" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B809" s="2" t="s">
+        <v>1552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change map renderer option number overlay to invisible in game
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20513DEA-B5DF-486E-A802-B801FBF5B070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927A49F5-8068-4020-9A92-579E2232B5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9400" yWindow="5600" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4827,9 +4827,6 @@
     <t>当前光照</t>
   </si>
   <si>
-    <t>使用数字渲染透明覆盖物</t>
-  </si>
-  <si>
     <t>标记矿物</t>
   </si>
   <si>
@@ -4848,10 +4845,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>MapRendererDlgInvisibleOverlay</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>MapRendererDlgDominatorLighting</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -4989,6 +4982,12 @@
   <si>
     <t>文件格式</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapRendererDlgInvisibleInGame</t>
+  </si>
+  <si>
+    <t>显示游戏内不可见对象</t>
   </si>
 </sst>
 </file>
@@ -5372,8 +5371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A797" workbookViewId="0">
-      <selection activeCell="B809" sqref="B809"/>
+    <sheetView tabSelected="1" topLeftCell="A794" workbookViewId="0">
+      <selection activeCell="A792" sqref="A792:XFD792"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10137,7 +10136,7 @@
         <v>1124</v>
       </c>
       <c r="B597" s="2" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
@@ -11045,7 +11044,7 @@
         <v>1336</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
@@ -11621,7 +11620,7 @@
         <v>1496</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.3">
@@ -11650,7 +11649,7 @@
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A786" s="2" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="B786" s="2" t="s">
         <v>1506</v>
@@ -11658,7 +11657,7 @@
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A787" s="2" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="B787" s="2" t="s">
         <v>1507</v>
@@ -11666,7 +11665,7 @@
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A788" s="2" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="B788" s="2" t="s">
         <v>486</v>
@@ -11674,7 +11673,7 @@
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A789" s="2" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="B789" s="2" t="s">
         <v>488</v>
@@ -11682,7 +11681,7 @@
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A790" s="2" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="B790" s="2" t="s">
         <v>490</v>
@@ -11690,7 +11689,7 @@
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A791" s="2" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="B791" s="2" t="s">
         <v>492</v>
@@ -11698,23 +11697,23 @@
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A792" s="2" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>1508</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A793" s="2" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>1521</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A794" s="2" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="B794" s="2" t="s">
         <v>1509</v>
@@ -11722,42 +11721,42 @@
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A795" s="2" t="s">
-        <v>1511</v>
+        <v>1520</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>1510</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A796" s="2" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B796" s="2" t="s">
         <v>1522</v>
-      </c>
-      <c r="B796" s="2" t="s">
-        <v>1523</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A797" s="2" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A798" s="2" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A799" s="2" t="s">
-        <v>1527</v>
+        <v>1529</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>1526</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.3">
@@ -11770,42 +11769,42 @@
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A801" s="2" t="s">
-        <v>1533</v>
+        <v>1541</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>1532</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A802" s="2" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="B802" s="2" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A803" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B803" s="2" t="s">
         <v>1536</v>
-      </c>
-    </row>
-    <row r="803" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A803" s="2" t="s">
-        <v>1542</v>
-      </c>
-      <c r="B803" s="2" t="s">
-        <v>1537</v>
       </c>
     </row>
     <row r="804" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A804" s="2" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="805" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="805" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A805" s="2" t="s">
-        <v>1540</v>
+        <v>1542</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>1539</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.3">
@@ -11826,10 +11825,10 @@
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A808" s="2" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
remove imageServer, improve building rendering
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927A49F5-8068-4020-9A92-579E2232B5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0C4EB5-D112-4405-A932-296260C3DED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="5600" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="3660" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="1553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="1549">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3594,14 +3594,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>LaunchImageServerFailed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法启动图像服务器！\n请检查ImageServer.exe是否存在，\n或关闭LoadImageDataFromServer。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Allhouse</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3716,9 +3708,6 @@
     <t>使用双线性插值缩放绘图界面(更精细，但更卡)</t>
   </si>
   <si>
-    <t>使用独立服务器进程存储游戏素材</t>
-  </si>
-  <si>
     <t>不将所属方翻译为其UIName</t>
   </si>
   <si>
@@ -3968,10 +3957,6 @@
   </si>
   <si>
     <t>Options.DDrawScalingBilinear</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.LoadImageDataFromServer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -5369,10 +5354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D809"/>
+  <dimension ref="A1:D807"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A794" workbookViewId="0">
-      <selection activeCell="A792" sqref="A792:XFD792"/>
+    <sheetView tabSelected="1" topLeftCell="A640" workbookViewId="0">
+      <selection activeCell="A655" sqref="A655:XFD655"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -7123,7 +7108,7 @@
         <v>411</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -7331,7 +7316,7 @@
         <v>462</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -7611,7 +7596,7 @@
         <v>531</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -7851,7 +7836,7 @@
         <v>579</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -7931,7 +7916,7 @@
         <v>598</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -7939,7 +7924,7 @@
         <v>599</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -7947,7 +7932,7 @@
         <v>600</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -7955,7 +7940,7 @@
         <v>601</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -7963,7 +7948,7 @@
         <v>602</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -7971,7 +7956,7 @@
         <v>603</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -8155,7 +8140,7 @@
         <v>644</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -8219,7 +8204,7 @@
         <v>658</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="70" x14ac:dyDescent="0.3">
@@ -8747,7 +8732,7 @@
         <v>778</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
@@ -10136,7 +10121,7 @@
         <v>1124</v>
       </c>
       <c r="B597" s="2" t="s">
-        <v>1548</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
@@ -10275,7 +10260,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="615" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A615" s="2" t="s">
         <v>1156</v>
       </c>
@@ -10285,654 +10270,654 @@
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A616" s="2" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="B616" s="2" t="s">
-        <v>1159</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A617" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B617" s="2" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A618" s="2" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B618" s="2" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A619" s="2" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B619" s="2" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A620" s="2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B620" s="2" t="s">
         <v>1165</v>
-      </c>
-      <c r="B618" s="2" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="619" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A619" s="2" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B619" s="2" t="s">
-        <v>1160</v>
-      </c>
-    </row>
-    <row r="620" spans="1:2" ht="35" x14ac:dyDescent="0.3">
-      <c r="A620" s="2" t="s">
-        <v>1231</v>
-      </c>
-      <c r="B620" s="2" t="s">
-        <v>1166</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" s="2" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="B621" s="2" t="s">
-        <v>1167</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="2" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>1355</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" s="2" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="B623" s="2" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="2" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" s="2" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="B625" s="2" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" s="2" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A627" s="2" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B627" s="2" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A628" s="2" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A629" s="2" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B629" s="2" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A630" s="2" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="B630" s="2" t="s">
-        <v>1175</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A631" s="2" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B631" s="2" t="s">
-        <v>1441</v>
-      </c>
+        <v>1305</v>
+      </c>
+      <c r="C631" s="4"/>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A632" s="2" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>1309</v>
+        <v>1438</v>
       </c>
       <c r="C632" s="4"/>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A633" s="2" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="B633" s="2" t="s">
-        <v>1442</v>
-      </c>
-      <c r="C633" s="4"/>
+        <v>1174</v>
+      </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A634" s="2" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B634" s="2" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A635" s="2" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="B635" s="2" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A636" s="2" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="B636" s="2" t="s">
-        <v>1178</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A637" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B637" s="2" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" ht="35" x14ac:dyDescent="0.3">
+      <c r="A638" s="2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B638" s="2" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A639" s="2" t="s">
         <v>1248</v>
       </c>
-      <c r="B637" s="2" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="638" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A638" s="2" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B638" s="2" t="s">
+      <c r="B639" s="2" t="s">
         <v>1179</v>
-      </c>
-    </row>
-    <row r="639" spans="1:3" ht="35" x14ac:dyDescent="0.3">
-      <c r="A639" s="2" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B639" s="2" t="s">
-        <v>1180</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A640" s="2" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" s="2" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="B641" s="2" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" s="2" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" s="2" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>1184</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" s="2" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" s="2" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="B645" s="2" t="s">
-        <v>1444</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" s="2" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>1185</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" s="2" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B647" s="2" t="s">
-        <v>1372</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" s="2" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" s="2" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="B649" s="2" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" s="2" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" s="2" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="B651" s="2" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" s="2" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" s="2" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="B653" s="2" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" s="2" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="2" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="B655" s="2" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" s="2" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A657" s="2" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B657" s="2" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A658" s="2" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A659" s="2" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>1197</v>
-      </c>
+        <v>1304</v>
+      </c>
+      <c r="C659" s="4"/>
+      <c r="D659" s="4"/>
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A660" s="2" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="661" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A661" s="2" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>1308</v>
-      </c>
-      <c r="C661" s="4"/>
-      <c r="D661" s="4"/>
+        <v>1197</v>
+      </c>
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A662" s="2" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="663" spans="1:4" ht="35" x14ac:dyDescent="0.3">
       <c r="A663" s="2" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A664" s="2" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B664" s="2" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="665" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A665" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B665" s="2" t="s">
         <v>1201</v>
-      </c>
-    </row>
-    <row r="665" spans="1:4" ht="35" x14ac:dyDescent="0.3">
-      <c r="A665" s="2" t="s">
-        <v>1276</v>
-      </c>
-      <c r="B665" s="2" t="s">
-        <v>1202</v>
       </c>
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A666" s="2" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>1203</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A667" s="2" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="B667" s="2" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A668" s="2" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>1329</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A669" s="2" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="670" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A670" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B670" s="2" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="671" spans="1:4" ht="35" x14ac:dyDescent="0.3">
+      <c r="A671" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B671" s="2" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="672" spans="1:4" ht="35" x14ac:dyDescent="0.3">
+      <c r="A672" s="2" t="s">
         <v>1281</v>
       </c>
-      <c r="B670" s="2" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="671" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A671" s="2" t="s">
+      <c r="B672" s="2" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A673" s="2" t="s">
         <v>1282</v>
       </c>
-      <c r="B671" s="2" t="s">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="672" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A672" s="2" t="s">
+      <c r="B673" s="2" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A674" s="2" t="s">
         <v>1283</v>
       </c>
-      <c r="B672" s="2" t="s">
-        <v>1208</v>
-      </c>
-    </row>
-    <row r="673" spans="1:2" ht="35" x14ac:dyDescent="0.3">
-      <c r="A673" s="2" t="s">
-        <v>1284</v>
-      </c>
-      <c r="B673" s="2" t="s">
+      <c r="B674" s="2" t="s">
         <v>1209</v>
-      </c>
-    </row>
-    <row r="674" spans="1:2" ht="35" x14ac:dyDescent="0.3">
-      <c r="A674" s="2" t="s">
-        <v>1285</v>
-      </c>
-      <c r="B674" s="2" t="s">
-        <v>1210</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675" s="2" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676" s="2" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677" s="2" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678" s="2" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679" s="2" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" s="2" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681" s="2" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682" s="2" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683" s="2" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684" s="2" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685" s="2" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>1221</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686" s="2" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687" s="2" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>1445</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688" s="2" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689" s="2" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690" s="2" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691" s="2" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>1226</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692" s="2" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="693" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A693" s="2" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>1446</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694" s="2" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="695" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A695" s="2" t="s">
         <v>1306</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>1229</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" s="2" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>1230</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.3">
@@ -10961,10 +10946,10 @@
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A700" s="2" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>1317</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.3">
@@ -10977,34 +10962,34 @@
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A702" s="2" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>1335</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703" s="2" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B703" s="2" t="s">
         <v>1322</v>
-      </c>
-      <c r="B703" s="2" t="s">
-        <v>1323</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704" s="2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B704" s="2" t="s">
         <v>1324</v>
-      </c>
-      <c r="B704" s="2" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705" s="2" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>1326</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
@@ -11015,60 +11000,60 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="707" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="707" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A707" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B707" s="2" t="s">
         <v>1330</v>
-      </c>
-      <c r="B707" s="2" t="s">
-        <v>1449</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708" s="2" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="B708" s="2" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="709" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A709" s="2" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B709" s="2" t="s">
         <v>1333</v>
-      </c>
-      <c r="B709" s="2" t="s">
-        <v>1334</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A710" s="2" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>1533</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A711" s="2" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A712" s="2" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A713" s="2" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>1339</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.3">
@@ -11081,10 +11066,10 @@
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A715" s="2" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B715" s="2" t="s">
         <v>1345</v>
-      </c>
-      <c r="B715" s="2" t="s">
-        <v>1346</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
@@ -11092,50 +11077,50 @@
         <v>1347</v>
       </c>
       <c r="B716" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A717" s="2" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A718" s="2" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>1350</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A719" s="2" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A720" s="2" t="s">
-        <v>1356</v>
+        <v>1369</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="721" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A721" s="2" t="s">
-        <v>1358</v>
+        <v>1372</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A722" s="2" t="s">
         <v>1373</v>
       </c>
@@ -11143,60 +11128,60 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="723" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+    <row r="723" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A723" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B723" s="2" t="s">
         <v>1376</v>
       </c>
-      <c r="B723" s="2" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="724" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A724" s="2" t="s">
-        <v>1377</v>
+        <v>1381</v>
       </c>
       <c r="B724" s="2" t="s">
-        <v>1378</v>
+        <v>165</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A725" s="2" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>1380</v>
+        <v>561</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>165</v>
+        <v>573</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A727" s="2" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>561</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A728" s="2" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B728" s="2" t="s">
         <v>1383</v>
-      </c>
-      <c r="B728" s="2" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A729" s="2" t="s">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>1381</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.3">
@@ -11249,26 +11234,26 @@
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A736" s="2" t="s">
-        <v>1398</v>
+        <v>1424</v>
       </c>
       <c r="B736" s="2" t="s">
-        <v>1399</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A737" s="2" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A738" s="2" t="s">
-        <v>1428</v>
+        <v>1400</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>1429</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.3">
@@ -11284,15 +11269,15 @@
         <v>1404</v>
       </c>
       <c r="B740" s="2" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A741" s="2" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="741" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A741" s="2" t="s">
+      <c r="B741" s="2" t="s">
         <v>1406</v>
-      </c>
-      <c r="B741" s="2" t="s">
-        <v>1407</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.3">
@@ -11300,12 +11285,12 @@
         <v>1408</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="743" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A743" s="2" t="s">
-        <v>1409</v>
+        <v>1419</v>
       </c>
       <c r="B743" s="2" t="s">
         <v>1410</v>
@@ -11313,50 +11298,50 @@
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A744" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B744" s="2" t="s">
         <v>1412</v>
-      </c>
-      <c r="B744" s="2" t="s">
-        <v>1413</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A745" s="2" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A746" s="2" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A747" s="2" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B748" s="2" t="s">
         <v>1420</v>
-      </c>
-      <c r="B748" s="2" t="s">
-        <v>1417</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A749" s="2" t="s">
-        <v>1419</v>
+        <v>1423</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>1418</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
@@ -11364,15 +11349,15 @@
         <v>1426</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>1424</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A751" s="2" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1425</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.3">
@@ -11396,76 +11381,76 @@
         <v>1434</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>1435</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A755" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B755" s="2" t="s">
         <v>1436</v>
       </c>
-      <c r="B755" s="2" t="s">
-        <v>1437</v>
-      </c>
-    </row>
-    <row r="756" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="756" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
       <c r="A756" s="2" t="s">
-        <v>1438</v>
+        <v>1454</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>1447</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A757" s="2" t="s">
-        <v>1439</v>
+        <v>1453</v>
       </c>
       <c r="B757" s="2" t="s">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="758" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A758" s="2" t="s">
-        <v>1458</v>
+        <v>1452</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>1459</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A759" s="2" t="s">
-        <v>1457</v>
+        <v>1451</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A760" s="2" t="s">
-        <v>1456</v>
+        <v>1450</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A761" s="2" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>1452</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A762" s="2" t="s">
-        <v>1454</v>
+        <v>1459</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>1453</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A763" s="2" t="s">
-        <v>1460</v>
+        <v>1464</v>
       </c>
       <c r="B763" s="2" t="s">
         <v>1461</v>
@@ -11476,12 +11461,12 @@
         <v>1463</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A765" s="2" t="s">
-        <v>1468</v>
+        <v>1470</v>
       </c>
       <c r="B765" s="2" t="s">
         <v>1465</v>
@@ -11489,7 +11474,7 @@
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A766" s="2" t="s">
-        <v>1467</v>
+        <v>1469</v>
       </c>
       <c r="B766" s="2" t="s">
         <v>1466</v>
@@ -11497,119 +11482,119 @@
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A767" s="2" t="s">
-        <v>1474</v>
+        <v>1468</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A768" s="2" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A769" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B769" s="2" t="s">
         <v>1472</v>
-      </c>
-      <c r="B769" s="2" t="s">
-        <v>1471</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A770" s="2" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A771" s="2" t="s">
-        <v>1479</v>
+        <v>1490</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A772" s="2" t="s">
-        <v>1480</v>
+        <v>1489</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A773" s="2" t="s">
-        <v>1494</v>
+        <v>1488</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A774" s="2" t="s">
-        <v>1493</v>
+        <v>1487</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A775" s="2" t="s">
-        <v>1492</v>
+        <v>1486</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A776" s="2" t="s">
-        <v>1491</v>
+        <v>1485</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A777" s="2" t="s">
-        <v>1490</v>
+        <v>1484</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A778" s="2" t="s">
-        <v>1489</v>
+        <v>1494</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>1486</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A779" s="2" t="s">
-        <v>1488</v>
+        <v>1493</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>1487</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A780" s="2" t="s">
-        <v>1498</v>
+        <v>1492</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>1505</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A781" s="2" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B781" s="2" t="s">
         <v>1495</v>
@@ -11617,186 +11602,186 @@
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A782" s="2" t="s">
-        <v>1496</v>
+        <v>1498</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>1532</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A783" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B783" s="2" t="s">
         <v>1500</v>
-      </c>
-      <c r="B783" s="2" t="s">
-        <v>1499</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A784" s="2" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B784" s="2" t="s">
         <v>1502</v>
-      </c>
-      <c r="B784" s="2" t="s">
-        <v>1501</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A785" s="2" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B785" s="2" t="s">
         <v>1503</v>
-      </c>
-      <c r="B785" s="2" t="s">
-        <v>1504</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A786" s="2" t="s">
-        <v>1518</v>
+        <v>1512</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>1506</v>
+        <v>486</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A787" s="2" t="s">
-        <v>1517</v>
+        <v>1511</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>1507</v>
+        <v>488</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A788" s="2" t="s">
-        <v>1516</v>
+        <v>1510</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A789" s="2" t="s">
-        <v>1515</v>
+        <v>1509</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A790" s="2" t="s">
-        <v>1514</v>
+        <v>1508</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>490</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A791" s="2" t="s">
-        <v>1513</v>
+        <v>1507</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>492</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A792" s="2" t="s">
-        <v>1512</v>
+        <v>1506</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>1519</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A793" s="2" t="s">
-        <v>1511</v>
+        <v>1516</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>1508</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A794" s="2" t="s">
-        <v>1510</v>
+        <v>1523</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>1509</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A795" s="2" t="s">
-        <v>1520</v>
+        <v>1522</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A796" s="2" t="s">
-        <v>1527</v>
+        <v>1521</v>
       </c>
       <c r="B796" s="2" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A797" s="2" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A798" s="2" t="s">
-        <v>1525</v>
+        <v>1527</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>1524</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A799" s="2" t="s">
-        <v>1529</v>
+        <v>1537</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>1528</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A800" s="2" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B800" s="2" t="s">
         <v>1531</v>
       </c>
-      <c r="B800" s="2" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="801" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="801" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A801" s="2" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B801" s="2" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A802" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B802" s="2" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A803" s="2" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B803" s="2" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="804" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A804" s="2" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B804" s="2" t="s">
         <v>1541</v>
-      </c>
-      <c r="B801" s="2" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="802" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A802" s="2" t="s">
-        <v>1540</v>
-      </c>
-      <c r="B802" s="2" t="s">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="803" spans="1:2" ht="35" x14ac:dyDescent="0.3">
-      <c r="A803" s="2" t="s">
-        <v>1539</v>
-      </c>
-      <c r="B803" s="2" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="804" spans="1:2" ht="35" x14ac:dyDescent="0.3">
-      <c r="A804" s="2" t="s">
-        <v>1538</v>
-      </c>
-      <c r="B804" s="2" t="s">
-        <v>1537</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.3">
@@ -11809,34 +11794,18 @@
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A806" s="2" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A807" s="2" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="808" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A808" s="2" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B808" s="2" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="809" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A809" s="2" t="s">
-        <v>1551</v>
-      </c>
-      <c r="B809" s="2" t="s">
-        <v>1552</v>
+        <v>1548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
random slope in random terrain generator
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92502779-0323-42EB-852C-49F926FA54DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10395474-C47A-4ED2-93FD-0E02726B3CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="930" windowWidth="21790" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="930" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="2292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="2304">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21029,6 +21029,79 @@
   <si>
     <t>Special</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lower height delta:</t>
+  </si>
+  <si>
+    <t>Heighten height delta:</t>
+  </si>
+  <si>
+    <t>Slope Smoothing (0-200):</t>
+  </si>
+  <si>
+    <t>Slopes</t>
+  </si>
+  <si>
+    <t>CTerrainGenerator.Slopes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeSteepness</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeMaxDelta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeMinDelta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>最大降低高度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>最大抬升高度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>起伏强度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(0-200):</t>
+    </r>
+  </si>
+  <si>
+    <t>斜坡</t>
   </si>
 </sst>
 </file>
@@ -21437,10 +21510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C814"/>
+  <dimension ref="A1:C818"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A802" workbookViewId="0">
-      <selection activeCell="A815" sqref="A815"/>
+    <sheetView tabSelected="1" topLeftCell="A792" workbookViewId="0">
+      <selection activeCell="B810" sqref="B810"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -30387,6 +30460,50 @@
         <v>2288</v>
       </c>
     </row>
+    <row r="815" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A815" s="4" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B815" s="5" t="s">
+        <v>2300</v>
+      </c>
+      <c r="C815" s="3" t="s">
+        <v>2292</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A816" s="4" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B816" s="5" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C816" s="3" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A817" s="4" t="s">
+        <v>2297</v>
+      </c>
+      <c r="B817" s="5" t="s">
+        <v>2302</v>
+      </c>
+      <c r="C817" s="3" t="s">
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A818" s="4" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B818" s="5" t="s">
+        <v>2303</v>
+      </c>
+      <c r="C818" s="3" t="s">
+        <v>2295</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add more functions to random slope
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10395474-C47A-4ED2-93FD-0E02726B3CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1702E7F3-A6FF-4ED2-B2D2-B9DED4DF9853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="930" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="2304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="2319">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21102,6 +21102,105 @@
   </si>
   <si>
     <t>斜坡</t>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeMarcoSteepness</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeManualHeight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeHeightTransition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeCoords</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeCoordHeights</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marco steepness (0-200):</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manually set base height:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height transition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start and end coords (x,y):</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start and end heights:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>宏观起伏</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(0-200):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>指定基础高度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>高度渐变</t>
+  </si>
+  <si>
+    <r>
+      <t>起始终结坐标</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(x,y):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>对应高度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -21510,10 +21609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C818"/>
+  <dimension ref="A1:C823"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A792" workbookViewId="0">
-      <selection activeCell="B810" sqref="B810"/>
+    <sheetView tabSelected="1" topLeftCell="A797" workbookViewId="0">
+      <selection activeCell="B813" sqref="B813"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -30460,7 +30559,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="815" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="815" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A815" s="4" t="s">
         <v>2299</v>
       </c>
@@ -30471,7 +30570,7 @@
         <v>2292</v>
       </c>
     </row>
-    <row r="816" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="816" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A816" s="4" t="s">
         <v>2298</v>
       </c>
@@ -30482,7 +30581,7 @@
         <v>2293</v>
       </c>
     </row>
-    <row r="817" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="817" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A817" s="4" t="s">
         <v>2297</v>
       </c>
@@ -30493,7 +30592,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="818" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="818" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A818" s="4" t="s">
         <v>2296</v>
       </c>
@@ -30502,6 +30601,61 @@
       </c>
       <c r="C818" s="3" t="s">
         <v>2295</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A819" s="4" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B819" s="5" t="s">
+        <v>2314</v>
+      </c>
+      <c r="C819" s="3" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A820" s="4" t="s">
+        <v>2305</v>
+      </c>
+      <c r="B820" s="5" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C820" s="3" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="821" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A821" s="4" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B821" s="5" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C821" s="3" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="822" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A822" s="4" t="s">
+        <v>2307</v>
+      </c>
+      <c r="B822" s="5" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C822" s="3" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="823" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A823" s="4" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B823" s="5" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C823" s="3" t="s">
+        <v>2313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more features for slope
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1702E7F3-A6FF-4ED2-B2D2-B9DED4DF9853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C6E8FC-07BE-4C38-A983-B42FBC4C9FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="930" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5310" yWindow="840" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="2319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2472" uniqueCount="2328">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21201,6 +21201,59 @@
       </rPr>
       <t>:</t>
     </r>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeMarcoMinDelta</t>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeMarcoMaxDelta</t>
+  </si>
+  <si>
+    <t>Marco Lower height delta:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marco Heighten height delta:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>宏观最大降低高度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>宏观最大抬升高度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeAvoidEdges</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avoid edges</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>避让选区边界</t>
   </si>
 </sst>
 </file>
@@ -21609,10 +21662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C823"/>
+  <dimension ref="A1:C826"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A797" workbookViewId="0">
-      <selection activeCell="B813" sqref="B813"/>
+    <sheetView tabSelected="1" topLeftCell="A810" workbookViewId="0">
+      <selection activeCell="C822" sqref="C822"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -30603,7 +30656,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="819" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="819" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A819" s="4" t="s">
         <v>2304</v>
       </c>
@@ -30614,7 +30667,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="820" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="820" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A820" s="4" t="s">
         <v>2305</v>
       </c>
@@ -30625,7 +30678,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="821" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="821" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A821" s="4" t="s">
         <v>2306</v>
       </c>
@@ -30636,7 +30689,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="822" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="822" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A822" s="4" t="s">
         <v>2307</v>
       </c>
@@ -30647,7 +30700,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="823" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="823" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A823" s="4" t="s">
         <v>2308</v>
       </c>
@@ -30656,6 +30709,39 @@
       </c>
       <c r="C823" s="3" t="s">
         <v>2313</v>
+      </c>
+    </row>
+    <row r="824" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A824" s="4" t="s">
+        <v>2319</v>
+      </c>
+      <c r="B824" s="5" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C824" s="3" t="s">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="825" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A825" s="4" t="s">
+        <v>2320</v>
+      </c>
+      <c r="B825" s="5" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C825" s="3" t="s">
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="826" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A826" s="4" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B826" s="5" t="s">
+        <v>2327</v>
+      </c>
+      <c r="C826" s="3" t="s">
+        <v>2326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support custom wp & celltag color, fix GetAvailableIndex bug
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C6E8FC-07BE-4C38-A983-B42FBC4C9FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B674F6-B384-4727-A13A-C3E7C84F3511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="840" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14210" yWindow="950" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2472" uniqueCount="2328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2487" uniqueCount="2343">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21254,6 +21254,56 @@
   </si>
   <si>
     <t>避让选区边界</t>
+  </si>
+  <si>
+    <t>Draw celltags translucently</t>
+  </si>
+  <si>
+    <t>Set waypoint color</t>
+  </si>
+  <si>
+    <t>Remove waypoint color</t>
+  </si>
+  <si>
+    <t>Set celltag color</t>
+  </si>
+  <si>
+    <t>Remove celltag color</t>
+  </si>
+  <si>
+    <t>RemoveCelltagColorObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetCelltagColorObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemoveWaypColorObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetWaypColorObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DrawCelltagTranslucent</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>半透明绘制单元标记</t>
+  </si>
+  <si>
+    <t>设置路径点颜色</t>
+  </si>
+  <si>
+    <t>移除路径点颜色</t>
+  </si>
+  <si>
+    <t>设置单元标记颜色</t>
+  </si>
+  <si>
+    <t>移除单元标记颜色</t>
   </si>
 </sst>
 </file>
@@ -21662,10 +21712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C826"/>
+  <dimension ref="A1:C831"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A810" workbookViewId="0">
-      <selection activeCell="C822" sqref="C822"/>
+      <selection activeCell="B825" sqref="B825"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -30733,7 +30783,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="826" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="826" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A826" s="4" t="s">
         <v>2325</v>
       </c>
@@ -30742,6 +30792,61 @@
       </c>
       <c r="C826" s="3" t="s">
         <v>2326</v>
+      </c>
+    </row>
+    <row r="827" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A827" s="4" t="s">
+        <v>2337</v>
+      </c>
+      <c r="B827" s="5" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C827" s="3" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="828" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A828" s="4" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B828" s="5" t="s">
+        <v>2339</v>
+      </c>
+      <c r="C828" s="3" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="829" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A829" s="4" t="s">
+        <v>2335</v>
+      </c>
+      <c r="B829" s="5" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C829" s="3" t="s">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="830" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A830" s="4" t="s">
+        <v>2334</v>
+      </c>
+      <c r="B830" s="5" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C830" s="3" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="831" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A831" s="4" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B831" s="5" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C831" s="3" t="s">
+        <v>2332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support turret shadow, fix shadow position, fix city cliff draw
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B674F6-B384-4727-A13A-C3E7C84F3511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1579CD68-96F6-47EB-B81D-E6B6D77B7911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14210" yWindow="950" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2487" uniqueCount="2343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="2349">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21304,6 +21304,46 @@
   </si>
   <si>
     <t>移除单元标记颜色</t>
+  </si>
+  <si>
+    <t>Display voxel shadow on the ground instead of bottom</t>
+  </si>
+  <si>
+    <t>在地面上而不是体素的最底部渲染阴影</t>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Shadow.OnGround</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTerrainGenerator.SlopeDescription</t>
+  </si>
+  <si>
+    <r>
+      <t>本工具生成随机斜坡地形。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>地形高度由两层起伏叠加而成：左侧参数控制局部细节起伏，影响地面陡峭程度；右侧宏观参数控制大尺度整体起伏，影响区域间的高低变化。最终效果为两者叠加。</t>
+    </r>
+  </si>
+  <si>
+    <t>This tool generates random sloped terrain.\nFinal height is composed of two layers: Left parameters control local detail variation and surface steepness. Right Marco parameters control large-scale elevation variation across the area. The final terrain is the combination of both layers.</t>
   </si>
 </sst>
 </file>
@@ -21712,10 +21752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C831"/>
+  <dimension ref="A1:C833"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A810" workbookViewId="0">
-      <selection activeCell="B825" sqref="B825"/>
+    <sheetView tabSelected="1" topLeftCell="A824" workbookViewId="0">
+      <selection activeCell="C827" sqref="C827"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -30794,7 +30834,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="827" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="827" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A827" s="4" t="s">
         <v>2337</v>
       </c>
@@ -30805,7 +30845,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="828" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="828" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A828" s="4" t="s">
         <v>2336</v>
       </c>
@@ -30816,7 +30856,7 @@
         <v>2329</v>
       </c>
     </row>
-    <row r="829" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="829" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A829" s="4" t="s">
         <v>2335</v>
       </c>
@@ -30827,7 +30867,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="830" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="830" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A830" s="4" t="s">
         <v>2334</v>
       </c>
@@ -30838,7 +30878,7 @@
         <v>2331</v>
       </c>
     </row>
-    <row r="831" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="831" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A831" s="4" t="s">
         <v>2333</v>
       </c>
@@ -30847,6 +30887,28 @@
       </c>
       <c r="C831" s="3" t="s">
         <v>2332</v>
+      </c>
+    </row>
+    <row r="832" spans="1:3" ht="38" x14ac:dyDescent="0.4">
+      <c r="A832" s="4" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B832" s="5" t="s">
+        <v>2344</v>
+      </c>
+      <c r="C832" s="3" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="833" spans="1:3" ht="76" x14ac:dyDescent="0.4">
+      <c r="A833" s="4" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B833" s="5" t="s">
+        <v>2347</v>
+      </c>
+      <c r="C833" s="3" t="s">
+        <v>2348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimize mix loader, add reset default for paste options
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1579CD68-96F6-47EB-B81D-E6B6D77B7911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E88C767-C5D4-4BE7-903D-FB1A2518216C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="2349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="2352">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21344,6 +21344,17 @@
   </si>
   <si>
     <t>This tool generates random sloped terrain.\nFinal height is composed of two layers: Left parameters control local detail variation and surface steepness. Right Marco parameters control large-scale elevation variation across the area. The final terrain is the combination of both layers.</t>
+  </si>
+  <si>
+    <t>Menu.Paste.Reset</t>
+  </si>
+  <si>
+    <t>恢复默认</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset default</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -21752,10 +21763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C833"/>
+  <dimension ref="A1:C834"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A824" workbookViewId="0">
-      <selection activeCell="C827" sqref="C827"/>
+      <selection activeCell="C833" sqref="C833"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -30900,7 +30911,7 @@
         <v>2343</v>
       </c>
     </row>
-    <row r="833" spans="1:3" ht="76" x14ac:dyDescent="0.4">
+    <row r="833" spans="1:3" ht="95" x14ac:dyDescent="0.4">
       <c r="A833" s="4" t="s">
         <v>2346</v>
       </c>
@@ -30909,6 +30920,17 @@
       </c>
       <c r="C833" s="3" t="s">
         <v>2348</v>
+      </c>
+    </row>
+    <row r="834" spans="1:3" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A834" s="4" t="s">
+        <v>2349</v>
+      </c>
+      <c r="B834" s="5" t="s">
+        <v>2350</v>
+      </c>
+      <c r="C834" s="3" t="s">
+        <v>2351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support new actions of phobos
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E88C767-C5D4-4BE7-903D-FB1A2518216C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397EFD6C-9BE8-490C-A5B9-FF0C1693B762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="2352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="2353">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21354,6 +21354,10 @@
   </si>
   <si>
     <t>Reset default</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Waypoint</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -21765,8 +21769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C834"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A824" workbookViewId="0">
-      <selection activeCell="C833" sqref="C833"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -22430,7 +22434,7 @@
         <v>1191</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>2075</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
can keep map comments
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B391B51-0930-46E1-99CB-4827773036A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5DD18C-3AC5-4682-872D-FEE82914BE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="2353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="2356">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21411,6 +21411,16 @@
   <si>
     <t>This map contains include INIs. All key value pairs in the INIs will not be saved to the map, nor will be saved to the INIs.\nIf you click 'OK', this warning will no longer pop up in this map.\nNote: This feature is experimental and it is not recommended to use include within the map.</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.KeepComments</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keep existing map comments</t>
+  </si>
+  <si>
+    <t>保存地图时保留注释</t>
   </si>
 </sst>
 </file>
@@ -21832,10 +21842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C834"/>
+  <dimension ref="A1:C835"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A552" workbookViewId="0">
-      <selection activeCell="J554" sqref="J554"/>
+    <sheetView tabSelected="1" topLeftCell="A833" workbookViewId="0">
+      <selection activeCell="C834" sqref="C834"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
@@ -31002,6 +31012,17 @@
         <v>2347</v>
       </c>
     </row>
+    <row r="835" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A835" s="4" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B835" s="5" t="s">
+        <v>2355</v>
+      </c>
+      <c r="C835" s="3" t="s">
+        <v>2354</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
can open up to 10 trigger editor; can drag input params
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0908E69B-7432-489D-98C5-84B3603FC882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A5918B-7111-4D9D-9155-2AA1EDAC9552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="2365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="2400">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21453,6 +21453,119 @@
   </si>
   <si>
     <t>Options.PlaceStructure.PlaceUpgrade</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerOpenNewEditor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>多开编辑器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>New editor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerNewShort</t>
+  </si>
+  <si>
+    <t>新</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TriggerPlaceOnMapShort</t>
+  </si>
+  <si>
+    <t>放置</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>TriggerDisabledShort</t>
+  </si>
+  <si>
+    <t>禁</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>TriggerEasyShort</t>
+  </si>
+  <si>
+    <t>简</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>TriggerMediumShort</t>
+  </si>
+  <si>
+    <t>普</t>
+  </si>
+  <si>
+    <t>TriggerHardShort</t>
+  </si>
+  <si>
+    <t>困</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>TriggerAddShort</t>
+  </si>
+  <si>
+    <t>TriggerCloneShort</t>
+  </si>
+  <si>
+    <t>复</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>TriggerDeleteShort</t>
+  </si>
+  <si>
+    <t>删</t>
+  </si>
+  <si>
+    <t>SearchReferenceTitleShort</t>
+  </si>
+  <si>
+    <t>查找</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>紧凑模式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerCompactMode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compact Mode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerCompactModeShort</t>
+  </si>
+  <si>
+    <t>紧凑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compact</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -21859,10 +21972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C838"/>
+  <dimension ref="A1:C851"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A828" workbookViewId="0">
-      <selection activeCell="C834" sqref="C834"/>
+    <sheetView tabSelected="1" topLeftCell="A833" workbookViewId="0">
+      <selection activeCell="C851" sqref="A850:C851"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -31073,6 +31186,149 @@
         <v>2362</v>
       </c>
     </row>
+    <row r="839" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A839" s="4" t="s">
+        <v>2365</v>
+      </c>
+      <c r="B839" s="5" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C839" s="3" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="840" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A840" s="4" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B840" s="5" t="s">
+        <v>2369</v>
+      </c>
+      <c r="C840" s="3" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="841" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A841" s="4" t="s">
+        <v>2371</v>
+      </c>
+      <c r="B841" s="5" t="s">
+        <v>2372</v>
+      </c>
+      <c r="C841" s="3" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="842" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A842" s="4" t="s">
+        <v>2374</v>
+      </c>
+      <c r="B842" s="5" t="s">
+        <v>2375</v>
+      </c>
+      <c r="C842" s="3" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="843" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A843" s="4" t="s">
+        <v>2377</v>
+      </c>
+      <c r="B843" s="5" t="s">
+        <v>2378</v>
+      </c>
+      <c r="C843" s="3" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="844" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A844" s="4" t="s">
+        <v>2380</v>
+      </c>
+      <c r="B844" s="5" t="s">
+        <v>2381</v>
+      </c>
+      <c r="C844" s="3" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="845" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A845" s="4" t="s">
+        <v>2382</v>
+      </c>
+      <c r="B845" s="5" t="s">
+        <v>2383</v>
+      </c>
+      <c r="C845" s="3" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="846" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A846" s="4" t="s">
+        <v>2385</v>
+      </c>
+      <c r="B846" s="5" t="s">
+        <v>2369</v>
+      </c>
+      <c r="C846" s="3" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="847" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A847" s="4" t="s">
+        <v>2386</v>
+      </c>
+      <c r="B847" s="5" t="s">
+        <v>2387</v>
+      </c>
+      <c r="C847" s="3" t="s">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="848" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A848" s="4" t="s">
+        <v>2389</v>
+      </c>
+      <c r="B848" s="5" t="s">
+        <v>2390</v>
+      </c>
+      <c r="C848" s="3" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="849" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A849" s="4" t="s">
+        <v>2391</v>
+      </c>
+      <c r="B849" s="5" t="s">
+        <v>2392</v>
+      </c>
+      <c r="C849" s="3" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="850" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A850" s="4" t="s">
+        <v>2395</v>
+      </c>
+      <c r="B850" s="5" t="s">
+        <v>2394</v>
+      </c>
+      <c r="C850" s="3" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="851" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A851" s="4" t="s">
+        <v>2397</v>
+      </c>
+      <c r="B851" s="5" t="s">
+        <v>2398</v>
+      </c>
+      <c r="C851" s="3" t="s">
+        <v>2399</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support dot dragging for team, taskforce & script
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A5918B-7111-4D9D-9155-2AA1EDAC9552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1C52B2-1D6E-46A5-871D-983C8CB59765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="2400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2556" uniqueCount="2409">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21567,6 +21567,37 @@
   <si>
     <t>Compact</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DragAttachTag</t>
+  </si>
+  <si>
+    <t>Attaching tag: %s (%s)</t>
+  </si>
+  <si>
+    <t>附加标签: %s (%s)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>已有标签: %s (%s)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DragAttachPreviousTag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Previous tag: %s (%s)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DragAttachPreviousTagNone</t>
+  </si>
+  <si>
+    <t>Previous tag: %s</t>
+  </si>
+  <si>
+    <t>已有标签: %s</t>
   </si>
 </sst>
 </file>
@@ -21972,10 +22003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C851"/>
+  <dimension ref="A1:C854"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A833" workbookViewId="0">
-      <selection activeCell="C851" sqref="A850:C851"/>
+      <selection activeCell="C854" sqref="A854:C854"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -31329,6 +31360,39 @@
         <v>2399</v>
       </c>
     </row>
+    <row r="852" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A852" s="4" t="s">
+        <v>2400</v>
+      </c>
+      <c r="B852" s="5" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C852" s="3" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="853" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A853" s="4" t="s">
+        <v>2404</v>
+      </c>
+      <c r="B853" s="5" t="s">
+        <v>2403</v>
+      </c>
+      <c r="C853" s="3" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="854" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A854" s="4" t="s">
+        <v>2406</v>
+      </c>
+      <c r="B854" s="5" t="s">
+        <v>2408</v>
+      </c>
+      <c r="C854" s="3" t="s">
+        <v>2407</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
display properties when using property brush
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1C52B2-1D6E-46A5-871D-983C8CB59765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5D743-8FAC-44A2-9EF2-85AC8BED073E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1370" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2990" yWindow="1260" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2556" uniqueCount="2409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="2465">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21570,34 +21570,248 @@
   </si>
   <si>
     <t>DragAttachTag</t>
-  </si>
-  <si>
-    <t>Attaching tag: %s (%s)</t>
-  </si>
-  <si>
-    <t>附加标签: %s (%s)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>已有标签: %s (%s)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DragAttachPreviousTag</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Previous tag: %s (%s)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DragAttachPreviousTagNone</t>
-  </si>
-  <si>
-    <t>Previous tag: %s</t>
-  </si>
-  <si>
-    <t>已有标签: %s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>标签: %s -&gt; %s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag: %s -&gt; %s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.Upgrade2</t>
+  </si>
+  <si>
+    <t>PropertyBrush.Upgrade3</t>
+  </si>
+  <si>
+    <t>PropertyBrush.House</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.Health</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>PropertyBrush.Facing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facing</t>
+  </si>
+  <si>
+    <t>PropertyBrush.AISellable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AISellable</t>
+  </si>
+  <si>
+    <t>PropertyBrush.PoweredOn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.AIRebuildable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIRebuildable</t>
+  </si>
+  <si>
+    <t>PoweredOn</t>
+  </si>
+  <si>
+    <t>PropertyBrush.Upgrades</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upgrades</t>
+  </si>
+  <si>
+    <t>PropertyBrush.SpotLight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpotLight</t>
+  </si>
+  <si>
+    <t>PropertyBrush.Upgrade1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upgrade1</t>
+  </si>
+  <si>
+    <t>Upgrade2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIRepairable</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Upgrade3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.AIRepairable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.Nominal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.Tag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.VeterancyPercentage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Veterancy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.Group</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.IsAboveGround</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsAboveGround</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.AutoNORecruitType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AutoNORecruitType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.AutoYESRecruitType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AutoYESRecruitType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PropertyBrush.FollowsIndex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FollowsIndex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属方</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>强度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>方向</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI变卖</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>重建</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>耗能/工作</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>组件数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>探照灯</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>组件1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>组件2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>组件3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI修复</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示名称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>标签</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>经验等级</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在桥梁上</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>重组A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>重组B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>跟随ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -22003,10 +22217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C854"/>
+  <dimension ref="A1:C873"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A833" workbookViewId="0">
-      <selection activeCell="C854" sqref="A854:C854"/>
+    <sheetView tabSelected="1" topLeftCell="A850" workbookViewId="0">
+      <selection activeCell="B860" sqref="B860"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -31365,21 +31579,21 @@
         <v>2400</v>
       </c>
       <c r="B852" s="5" t="s">
+        <v>2401</v>
+      </c>
+      <c r="C852" s="3" t="s">
         <v>2402</v>
-      </c>
-      <c r="C852" s="3" t="s">
-        <v>2401</v>
       </c>
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A853" s="4" t="s">
-        <v>2404</v>
+        <v>2405</v>
       </c>
       <c r="B853" s="5" t="s">
-        <v>2403</v>
+        <v>2444</v>
       </c>
       <c r="C853" s="3" t="s">
-        <v>2405</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.4">
@@ -31387,10 +31601,219 @@
         <v>2406</v>
       </c>
       <c r="B854" s="5" t="s">
-        <v>2408</v>
+        <v>2445</v>
       </c>
       <c r="C854" s="3" t="s">
         <v>2407</v>
+      </c>
+    </row>
+    <row r="855" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A855" s="4" t="s">
+        <v>2408</v>
+      </c>
+      <c r="B855" s="5" t="s">
+        <v>2446</v>
+      </c>
+      <c r="C855" s="3" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="856" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A856" s="4" t="s">
+        <v>2410</v>
+      </c>
+      <c r="B856" s="5" t="s">
+        <v>2447</v>
+      </c>
+      <c r="C856" s="3" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="857" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A857" s="4" t="s">
+        <v>2413</v>
+      </c>
+      <c r="B857" s="5" t="s">
+        <v>2448</v>
+      </c>
+      <c r="C857" s="3" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="858" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A858" s="4" t="s">
+        <v>2412</v>
+      </c>
+      <c r="B858" s="5" t="s">
+        <v>2449</v>
+      </c>
+      <c r="C858" s="3" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="859" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A859" s="4" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B859" s="5" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C859" s="3" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="860" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A860" s="4" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B860" s="5" t="s">
+        <v>2451</v>
+      </c>
+      <c r="C860" s="3" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="861" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A861" s="4" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B861" s="5" t="s">
+        <v>2452</v>
+      </c>
+      <c r="C861" s="3" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="862" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A862" s="4" t="s">
+        <v>2403</v>
+      </c>
+      <c r="B862" s="5" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C862" s="3" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="863" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A863" s="4" t="s">
+        <v>2404</v>
+      </c>
+      <c r="B863" s="5" t="s">
+        <v>2454</v>
+      </c>
+      <c r="C863" s="3" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="864" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A864" s="4" t="s">
+        <v>2429</v>
+      </c>
+      <c r="B864" s="5" t="s">
+        <v>2455</v>
+      </c>
+      <c r="C864" s="3" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="865" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A865" s="4" t="s">
+        <v>2430</v>
+      </c>
+      <c r="B865" s="5" t="s">
+        <v>2456</v>
+      </c>
+      <c r="C865" s="3" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="866" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A866" s="4" t="s">
+        <v>2431</v>
+      </c>
+      <c r="B866" s="5" t="s">
+        <v>2457</v>
+      </c>
+      <c r="C866" s="3" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="867" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A867" s="4" t="s">
+        <v>2432</v>
+      </c>
+      <c r="B867" s="5" t="s">
+        <v>2458</v>
+      </c>
+      <c r="C867" s="3" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="868" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A868" s="4" t="s">
+        <v>2433</v>
+      </c>
+      <c r="B868" s="5" t="s">
+        <v>2459</v>
+      </c>
+      <c r="C868" s="3" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A869" s="4" t="s">
+        <v>2435</v>
+      </c>
+      <c r="B869" s="5" t="s">
+        <v>2460</v>
+      </c>
+      <c r="C869" s="3" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="870" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A870" s="4" t="s">
+        <v>2436</v>
+      </c>
+      <c r="B870" s="5" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C870" s="3" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="871" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A871" s="4" t="s">
+        <v>2438</v>
+      </c>
+      <c r="B871" s="5" t="s">
+        <v>2462</v>
+      </c>
+      <c r="C871" s="3" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="872" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A872" s="4" t="s">
+        <v>2440</v>
+      </c>
+      <c r="B872" s="5" t="s">
+        <v>2463</v>
+      </c>
+      <c r="C872" s="3" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="873" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A873" s="4" t="s">
+        <v>2442</v>
+      </c>
+      <c r="B873" s="5" t="s">
+        <v>2464</v>
+      </c>
+      <c r="C873" s="3" t="s">
+        <v>2443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduce Scintilla for better ini coding
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5D743-8FAC-44A2-9EF2-85AC8BED073E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39673F3-326C-4194-8DCD-54A0B267A138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2990" yWindow="1260" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="2465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="2468">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21811,6 +21811,18 @@
   </si>
   <si>
     <t>跟随ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FailedLoadScintillaDLL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Could not Load Scintilla.dll!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法加载Scintilla.dll!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -22217,10 +22229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C873"/>
+  <dimension ref="A1:C874"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A850" workbookViewId="0">
-      <selection activeCell="B860" sqref="B860"/>
+      <selection activeCell="B870" sqref="B870"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -31816,6 +31828,17 @@
         <v>2443</v>
       </c>
     </row>
+    <row r="874" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A874" s="4" t="s">
+        <v>2465</v>
+      </c>
+      <c r="B874" s="5" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C874" s="3" t="s">
+        <v>2466</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add batch trigger editor, fix custom tileset crash
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39673F3-326C-4194-8DCD-54A0B267A138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACB08CC-72AC-4173-882B-54C7F0564491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2990" yWindow="1260" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="2468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="2533">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21823,6 +21823,242 @@
   </si>
   <si>
     <t>无法加载Scintilla.dll!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerActionSplit</t>
+  </si>
+  <si>
+    <t>拆分</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Split</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatchTriggerTitle</t>
+  </si>
+  <si>
+    <t>BatchTriggerEventIndex</t>
+  </si>
+  <si>
+    <t>BatchTriggerActionIndex</t>
+  </si>
+  <si>
+    <t>BatchTriggerAdd</t>
+  </si>
+  <si>
+    <t>BatchTriggerRemove</t>
+  </si>
+  <si>
+    <t>BatchTriggerAutoFill</t>
+  </si>
+  <si>
+    <t>BatchTriggerUseID</t>
+  </si>
+  <si>
+    <t>BatchTriggerAllTriggers</t>
+  </si>
+  <si>
+    <t>BatchTriggerCurrentTriggers</t>
+  </si>
+  <si>
+    <t>BatchTriggerSearchTrigger</t>
+  </si>
+  <si>
+    <t>BatchTriggerDesc</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewID</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewName</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewEvent</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewAction</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP1</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP2</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP3</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP4</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP5</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP6</t>
+  </si>
+  <si>
+    <t>触发批量编辑器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件索引:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行为索引:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动填充</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有触发:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前触发:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索触发ID/名称:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>从左侧触发列表多选后，点击“添加”加入右侧栏目中。修改事件索引与行为索引以显示你需要修改的部分。双击任意单元格对目标参数进行修改。当在同一纵列中连续修改两个参数，且这两个参数存在可识别的递增规律（例如 TEST01 → TEST02），系统将自动按该规律推断并填充后续参数。默认显示参数对象的名称，勾选“使用ID”则显示其注册ID。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行为</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch Trigger Editor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event Index:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action Index:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Auto Fill</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All Triggers:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current Triggers:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search Trigger ID/Name:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select multiple triggers from the left list and click Add to include them in the right panel. Adjust the Event Index and Action Index to display the part you want to edit. Double-click any cell to modify the target parameter. When two consecutive parameters in the same column follow a recognizable incremental pattern (e.g. TEST01 → TEST02), the system will automatically infer the pattern and auto-fill subsequent values. By default, parameter names are shown, enable Use ID to display their registered IDs instead.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatchTriggerMoveUp</t>
+  </si>
+  <si>
+    <t>BatchTriggerMoveDown</t>
+  </si>
+  <si>
+    <t>上移</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下移</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Up</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Down</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -21830,7 +22066,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -21895,6 +22131,14 @@
       <family val="1"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -21928,7 +22172,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -21947,6 +22191,9 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -22229,10 +22476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C874"/>
+  <dimension ref="A1:C917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A850" workbookViewId="0">
-      <selection activeCell="B870" sqref="B870"/>
+    <sheetView tabSelected="1" topLeftCell="A881" workbookViewId="0">
+      <selection activeCell="A892" sqref="A892"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -31839,6 +32086,321 @@
         <v>2466</v>
       </c>
     </row>
+    <row r="875" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A875" s="4" t="s">
+        <v>2468</v>
+      </c>
+      <c r="B875" s="5" t="s">
+        <v>2469</v>
+      </c>
+      <c r="C875" s="3" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="876" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A876" s="4" t="s">
+        <v>2471</v>
+      </c>
+      <c r="B876" s="5" t="s">
+        <v>2492</v>
+      </c>
+      <c r="C876" s="3" t="s">
+        <v>2513</v>
+      </c>
+    </row>
+    <row r="877" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A877" s="4" t="s">
+        <v>2472</v>
+      </c>
+      <c r="B877" s="5" t="s">
+        <v>2493</v>
+      </c>
+      <c r="C877" s="3" t="s">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="878" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A878" s="4" t="s">
+        <v>2473</v>
+      </c>
+      <c r="B878" s="5" t="s">
+        <v>2494</v>
+      </c>
+      <c r="C878" s="3" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="879" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A879" s="4" t="s">
+        <v>2474</v>
+      </c>
+      <c r="B879" s="5" t="s">
+        <v>2495</v>
+      </c>
+      <c r="C879" s="3" t="s">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="880" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A880" s="4" t="s">
+        <v>2475</v>
+      </c>
+      <c r="B880" s="5" t="s">
+        <v>2496</v>
+      </c>
+      <c r="C880" s="3" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="881" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A881" s="4" t="s">
+        <v>2476</v>
+      </c>
+      <c r="B881" s="5" t="s">
+        <v>2497</v>
+      </c>
+      <c r="C881" s="3" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="882" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A882" s="4" t="s">
+        <v>2477</v>
+      </c>
+      <c r="B882" s="5" t="s">
+        <v>2498</v>
+      </c>
+      <c r="C882" s="3" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="883" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A883" s="4" t="s">
+        <v>2478</v>
+      </c>
+      <c r="B883" s="5" t="s">
+        <v>2499</v>
+      </c>
+      <c r="C883" s="3" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="884" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A884" s="4" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B884" s="5" t="s">
+        <v>2500</v>
+      </c>
+      <c r="C884" s="3" t="s">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="885" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A885" s="4" t="s">
+        <v>2480</v>
+      </c>
+      <c r="B885" s="5" t="s">
+        <v>2501</v>
+      </c>
+      <c r="C885" s="3" t="s">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="886" spans="1:3" ht="171" x14ac:dyDescent="0.4">
+      <c r="A886" s="4" t="s">
+        <v>2481</v>
+      </c>
+      <c r="B886" s="5" t="s">
+        <v>2502</v>
+      </c>
+      <c r="C886" s="3" t="s">
+        <v>2523</v>
+      </c>
+    </row>
+    <row r="887" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A887" s="4" t="s">
+        <v>2482</v>
+      </c>
+      <c r="B887" s="5" t="s">
+        <v>2503</v>
+      </c>
+      <c r="C887" s="3" t="s">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="888" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A888" s="4" t="s">
+        <v>2483</v>
+      </c>
+      <c r="B888" s="5" t="s">
+        <v>2504</v>
+      </c>
+      <c r="C888" s="3" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="889" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A889" s="4" t="s">
+        <v>2484</v>
+      </c>
+      <c r="B889" s="5" t="s">
+        <v>2505</v>
+      </c>
+      <c r="C889" s="3" t="s">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="890" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A890" s="4" t="s">
+        <v>2485</v>
+      </c>
+      <c r="B890" s="5" t="s">
+        <v>2506</v>
+      </c>
+      <c r="C890" s="3" t="s">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="891" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A891" s="4" t="s">
+        <v>2486</v>
+      </c>
+      <c r="B891" s="5" t="s">
+        <v>2507</v>
+      </c>
+      <c r="C891" s="3" t="s">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="892" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A892" s="4" t="s">
+        <v>2487</v>
+      </c>
+      <c r="B892" s="5" t="s">
+        <v>2508</v>
+      </c>
+      <c r="C892" s="3" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="893" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A893" s="4" t="s">
+        <v>2488</v>
+      </c>
+      <c r="B893" s="5" t="s">
+        <v>2509</v>
+      </c>
+      <c r="C893" s="3" t="s">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="894" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A894" s="4" t="s">
+        <v>2489</v>
+      </c>
+      <c r="B894" s="5" t="s">
+        <v>2510</v>
+      </c>
+      <c r="C894" s="3" t="s">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="895" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A895" s="4" t="s">
+        <v>2490</v>
+      </c>
+      <c r="B895" s="5" t="s">
+        <v>2511</v>
+      </c>
+      <c r="C895" s="3" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="896" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A896" s="4" t="s">
+        <v>2491</v>
+      </c>
+      <c r="B896" s="5" t="s">
+        <v>2512</v>
+      </c>
+      <c r="C896" s="3" t="s">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="897" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A897" s="4" t="s">
+        <v>2527</v>
+      </c>
+      <c r="B897" s="5" t="s">
+        <v>2529</v>
+      </c>
+      <c r="C897" s="3" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="898" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A898" s="4" t="s">
+        <v>2528</v>
+      </c>
+      <c r="B898" s="5" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C898" s="3" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="901" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A901" s="7"/>
+    </row>
+    <row r="902" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A902" s="7"/>
+    </row>
+    <row r="903" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A903" s="7"/>
+    </row>
+    <row r="904" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A904" s="7"/>
+    </row>
+    <row r="905" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A905" s="7"/>
+    </row>
+    <row r="906" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A906" s="7"/>
+    </row>
+    <row r="907" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A907" s="7"/>
+    </row>
+    <row r="908" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A908" s="7"/>
+    </row>
+    <row r="909" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A909" s="7"/>
+    </row>
+    <row r="910" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A910" s="7"/>
+    </row>
+    <row r="911" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A911" s="7"/>
+    </row>
+    <row r="912" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A912" s="7"/>
+    </row>
+    <row r="913" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A913" s="7"/>
+    </row>
+    <row r="914" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A914" s="7"/>
+    </row>
+    <row r="915" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A915" s="7"/>
+    </row>
+    <row r="916" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A916" s="7"/>
+    </row>
+    <row r="917" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A917" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
alt line tool support celltag, fix load comment bug
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACB08CC-72AC-4173-882B-54C7F0564491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555C21A6-D784-4163-A574-92B0C2E3B418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2990" yWindow="1260" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="2533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="2536">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -22059,6 +22059,17 @@
   </si>
   <si>
     <t>Down</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Edit.BatchTriggerEditor</t>
+  </si>
+  <si>
+    <t>Batch trigger editor\tCtrl+Alt+R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发批量编辑器\tCtrl+Alt+R</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -22479,7 +22490,7 @@
   <dimension ref="A1:C917"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A881" workbookViewId="0">
-      <selection activeCell="A892" sqref="A892"/>
+      <selection activeCell="C899" sqref="A899:C899"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -32350,6 +32361,17 @@
         <v>2532</v>
       </c>
     </row>
+    <row r="899" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A899" s="4" t="s">
+        <v>2533</v>
+      </c>
+      <c r="B899" s="5" t="s">
+        <v>2535</v>
+      </c>
+      <c r="C899" s="3" t="s">
+        <v>2534</v>
+      </c>
+    </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A901" s="7"/>
     </row>

</xml_diff>

<commit_message>
update batch editor style
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555C21A6-D784-4163-A574-92B0C2E3B418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8312692-C0F6-42BF-BD4E-BE3A1B11AFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2990" yWindow="1260" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="2536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="2545">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -21867,209 +21867,243 @@
     <t>BatchTriggerSearchTrigger</t>
   </si>
   <si>
+    <t>BatchTriggerViewID</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewName</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewEvent</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewAction</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP1</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP2</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP3</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP4</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP5</t>
+  </si>
+  <si>
+    <t>BatchTriggerViewP6</t>
+  </si>
+  <si>
+    <t>触发批量编辑器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件索引:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行为索引:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动填充</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有触发:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前触发:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索触发ID/名称:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行为</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch Trigger Editor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event Index:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action Index:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Auto Fill</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All Triggers:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current Triggers:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search Trigger ID/Name:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatchTriggerMoveUp</t>
+  </si>
+  <si>
+    <t>BatchTriggerMoveDown</t>
+  </si>
+  <si>
+    <t>上移</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下移</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Up</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Down</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Edit.BatchTriggerEditor</t>
+  </si>
+  <si>
+    <t>Batch trigger editor\tCtrl+Alt+R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发批量编辑器\tCtrl+Alt+R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatchTriggerDisplayID</t>
+  </si>
+  <si>
+    <t>显示ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatchTriggerHelp</t>
+  </si>
+  <si>
+    <t>帮助</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Help</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除高亮</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatchTriggerClearHighlight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clear Highlight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>BatchTriggerDesc</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewID</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewName</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewEvent</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewAction</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewP1</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewP2</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewP3</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewP4</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewP5</t>
-  </si>
-  <si>
-    <t>BatchTriggerViewP6</t>
-  </si>
-  <si>
-    <t>触发批量编辑器</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件索引:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>行为索引:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>移除</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>自动填充</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有触发:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>当前触发:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>搜索触发ID/名称:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>从左侧触发列表多选后，点击“添加”加入右侧栏目中。修改事件索引与行为索引以显示你需要修改的部分。双击任意单元格对目标参数进行修改。当在同一纵列中连续修改两个参数，且这两个参数存在可识别的递增规律（例如 TEST01 → TEST02），系统将自动按该规律推断并填充后续参数。默认显示参数对象的名称，勾选“使用ID”则显示其注册ID。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>行为</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Batch Trigger Editor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Event Index:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Action Index:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Add</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remove</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Auto Fill</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Use ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>All Triggers:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Current Triggers:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Search Trigger ID/Name:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Select multiple triggers from the left list and click Add to include them in the right panel. Adjust the Event Index and Action Index to display the part you want to edit. Double-click any cell to modify the target parameter. When two consecutive parameters in the same column follow a recognizable incremental pattern (e.g. TEST01 → TEST02), the system will automatically infer the pattern and auto-fill subsequent values. By default, parameter names are shown, enable Use ID to display their registered IDs instead.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Event</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Action</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BatchTriggerMoveUp</t>
-  </si>
-  <si>
-    <t>BatchTriggerMoveDown</t>
-  </si>
-  <si>
-    <t>上移</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>下移</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Up</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Down</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Menu.Edit.BatchTriggerEditor</t>
-  </si>
-  <si>
-    <t>Batch trigger editor\tCtrl+Alt+R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发批量编辑器\tCtrl+Alt+R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>从左侧触发列表多选后，点击“添加”加入右侧栏目中。仅有一个事件和行为会被显示，修改事件索引与行为索引以显示你需要修改的部分。双击任意单元格对目标参数进行修改。不论是否修改，被双击过的单元格都会呈现红色高亮状态。当在同一纵列中连续两个参数处于高亮，且这两个参数存在可识别的递增规律（例如 TEST01 → TEST02）时，点击“自动填充”，系统将自动按该规律推断并填充后续参数。点击“清除高亮”重置所有单元格的状态。默认显示触发、标签、小队参数的的名称，以数字方式显示路径点，勾选“使用ID”则显示其注册ID，以字母方式显示路径点。</t>
+  </si>
+  <si>
+    <t>After multi-selecting items from the trigger list on the left, click “Add” to move them into the column on the right. Only one event and behavior will be displayed. Change the event index and action index to display the part you want to modify. Double-click any cell to edit the target parameter. Regardless of whether changes are made, any cell that has been double-clicked will be highlighted in red. When two consecutive parameters in the same column are both highlighted and they follow a recognizable incremental pattern (for example, TEST01 → TEST02), click “Auto Fill”, and the system will automatically infer the pattern and fill in the subsequent parameters accordingly. Click “Clear Highlight” to reset the state of all cells. By default, the names of triggers, labels, and squad parameters are displayed, waypoints are shown numerically, and checking “Use ID” will display their registered IDs instead, with waypoints shown in letter format.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -22489,8 +22523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A881" workbookViewId="0">
-      <selection activeCell="C899" sqref="A899:C899"/>
+    <sheetView tabSelected="1" topLeftCell="A884" workbookViewId="0">
+      <selection activeCell="C886" sqref="C886"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -32113,10 +32147,10 @@
         <v>2471</v>
       </c>
       <c r="B876" s="5" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="C876" s="3" t="s">
-        <v>2513</v>
+        <v>2511</v>
       </c>
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.4">
@@ -32124,10 +32158,10 @@
         <v>2472</v>
       </c>
       <c r="B877" s="5" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="C877" s="3" t="s">
-        <v>2514</v>
+        <v>2512</v>
       </c>
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.4">
@@ -32135,10 +32169,10 @@
         <v>2473</v>
       </c>
       <c r="B878" s="5" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="C878" s="3" t="s">
-        <v>2515</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.4">
@@ -32146,10 +32180,10 @@
         <v>2474</v>
       </c>
       <c r="B879" s="5" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="C879" s="3" t="s">
-        <v>2516</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="880" spans="1:3" x14ac:dyDescent="0.4">
@@ -32157,10 +32191,10 @@
         <v>2475</v>
       </c>
       <c r="B880" s="5" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="C880" s="3" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.4">
@@ -32168,10 +32202,10 @@
         <v>2476</v>
       </c>
       <c r="B881" s="5" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="C881" s="3" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.4">
@@ -32179,10 +32213,10 @@
         <v>2477</v>
       </c>
       <c r="B882" s="5" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="C882" s="3" t="s">
-        <v>2519</v>
+        <v>2517</v>
       </c>
     </row>
     <row r="883" spans="1:3" x14ac:dyDescent="0.4">
@@ -32190,10 +32224,10 @@
         <v>2478</v>
       </c>
       <c r="B883" s="5" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="C883" s="3" t="s">
-        <v>2520</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.4">
@@ -32201,10 +32235,10 @@
         <v>2479</v>
       </c>
       <c r="B884" s="5" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="C884" s="3" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.4">
@@ -32212,192 +32246,198 @@
         <v>2480</v>
       </c>
       <c r="B885" s="5" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="C885" s="3" t="s">
-        <v>2522</v>
-      </c>
-    </row>
-    <row r="886" spans="1:3" ht="171" x14ac:dyDescent="0.4">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="886" spans="1:3" ht="285" x14ac:dyDescent="0.4">
       <c r="A886" s="4" t="s">
-        <v>2481</v>
+        <v>2542</v>
       </c>
       <c r="B886" s="5" t="s">
-        <v>2502</v>
+        <v>2543</v>
       </c>
       <c r="C886" s="3" t="s">
-        <v>2523</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A887" s="4" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="B887" s="5" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="C887" s="3" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A888" s="4" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="B888" s="5" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
       <c r="C888" s="3" t="s">
-        <v>2524</v>
+        <v>2521</v>
       </c>
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A889" s="4" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="B889" s="5" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
       <c r="C889" s="3" t="s">
-        <v>2525</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A890" s="4" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="B890" s="5" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
       <c r="C890" s="3" t="s">
-        <v>2526</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A891" s="4" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="B891" s="5" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
       <c r="C891" s="3" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="892" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A892" s="4" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="B892" s="5" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
       <c r="C892" s="3" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="893" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A893" s="4" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="B893" s="5" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
       <c r="C893" s="3" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A894" s="4" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="B894" s="5" t="s">
-        <v>2510</v>
+        <v>2508</v>
       </c>
       <c r="C894" s="3" t="s">
-        <v>2510</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="895" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A895" s="4" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="B895" s="5" t="s">
-        <v>2511</v>
+        <v>2509</v>
       </c>
       <c r="C895" s="3" t="s">
-        <v>2511</v>
+        <v>2509</v>
       </c>
     </row>
     <row r="896" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A896" s="4" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="B896" s="5" t="s">
-        <v>2512</v>
+        <v>2510</v>
       </c>
       <c r="C896" s="3" t="s">
-        <v>2512</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="897" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A897" s="4" t="s">
-        <v>2527</v>
+        <v>2524</v>
       </c>
       <c r="B897" s="5" t="s">
-        <v>2529</v>
+        <v>2526</v>
       </c>
       <c r="C897" s="3" t="s">
-        <v>2531</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="898" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A898" s="4" t="s">
-        <v>2528</v>
+        <v>2525</v>
       </c>
       <c r="B898" s="5" t="s">
-        <v>2530</v>
+        <v>2527</v>
       </c>
       <c r="C898" s="3" t="s">
-        <v>2532</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A899" s="4" t="s">
+        <v>2530</v>
+      </c>
+      <c r="B899" s="5" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C899" s="3" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A900" s="4" t="s">
         <v>2533</v>
       </c>
-      <c r="B899" s="5" t="s">
+      <c r="B900" s="5" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C900" s="3" t="s">
         <v>2535</v>
       </c>
-      <c r="C899" s="3" t="s">
-        <v>2534</v>
-      </c>
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A901" s="7"/>
+      <c r="A901" s="4" t="s">
+        <v>2536</v>
+      </c>
+      <c r="B901" s="5" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C901" s="3" t="s">
+        <v>2538</v>
+      </c>
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A902" s="7"/>
-    </row>
-    <row r="903" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A903" s="7"/>
-    </row>
-    <row r="904" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A904" s="7"/>
-    </row>
-    <row r="905" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A905" s="7"/>
-    </row>
-    <row r="906" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A906" s="7"/>
-    </row>
-    <row r="907" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A907" s="7"/>
-    </row>
-    <row r="908" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A908" s="7"/>
-    </row>
-    <row r="909" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A909" s="7"/>
+      <c r="A902" s="4" t="s">
+        <v>2540</v>
+      </c>
+      <c r="B902" s="5" t="s">
+        <v>2539</v>
+      </c>
+      <c r="C902" s="3" t="s">
+        <v>2541</v>
+      </c>
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A910" s="7"/>

</xml_diff>

<commit_message>
support default image, custom insignia
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8312692-C0F6-42BF-BD4E-BE3A1B11AFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8367F47-300E-4DD7-8125-DA8DFB504165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2990" yWindow="1260" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="2280" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="2545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="2548">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -22105,6 +22105,16 @@
   <si>
     <t>After multi-selecting items from the trigger list on the left, click “Add” to move them into the column on the right. Only one event and behavior will be displayed. Change the event index and action index to display the part you want to modify. Double-click any cell to edit the target parameter. Regardless of whether changes are made, any cell that has been double-clicked will be highlighted in red. When two consecutive parameters in the same column are both highlighted and they follow a recognizable incremental pattern (for example, TEST01 → TEST02), click “Auto Fill”, and the system will automatically infer the pattern and fill in the subsequent parameters accordingly. Click “Clear Highlight” to reset the state of all cells. By default, the names of triggers, labels, and squad parameters are displayed, waypoints are shown numerically, and checking “Use ID” will display their registered IDs instead, with waypoints shown in letter format.</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UseDefaultUnitImage</t>
+  </si>
+  <si>
+    <t>Display default images for vehicles, infantry, aircraft without images</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>为没有图像的车辆、步兵与飞行器显示缺省图像</t>
   </si>
 </sst>
 </file>
@@ -22523,8 +22533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A884" workbookViewId="0">
-      <selection activeCell="C886" sqref="C886"/>
+    <sheetView tabSelected="1" topLeftCell="A894" workbookViewId="0">
+      <selection activeCell="B903" sqref="B903"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -32439,6 +32449,17 @@
         <v>2541</v>
       </c>
     </row>
+    <row r="903" spans="1:3" ht="38" x14ac:dyDescent="0.4">
+      <c r="A903" s="4" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B903" s="5" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C903" s="3" t="s">
+        <v>2546</v>
+      </c>
+    </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A910" s="7"/>
     </row>

</xml_diff>

<commit_message>
add options to display default image for techno attachments
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8367F47-300E-4DD7-8125-DA8DFB504165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA7B0AE-1790-4255-8E20-1D2EF5FBA30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="2280" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="2548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2706" uniqueCount="2551">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -22115,6 +22115,18 @@
   </si>
   <si>
     <t>为没有图像的车辆、步兵与飞行器显示缺省图像</t>
+  </si>
+  <si>
+    <t>Options.UseDefaultUnitImage.TechnoAttachment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display default images for techno attachments without images</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>为没有图像的附加单位显示缺省图像</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -22534,7 +22546,7 @@
   <dimension ref="A1:C917"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A894" workbookViewId="0">
-      <selection activeCell="B903" sqref="B903"/>
+      <selection activeCell="C904" sqref="A904:C904"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -32460,6 +32472,17 @@
         <v>2546</v>
       </c>
     </row>
+    <row r="904" spans="1:3" ht="38" x14ac:dyDescent="0.4">
+      <c r="A904" s="4" t="s">
+        <v>2548</v>
+      </c>
+      <c r="B904" s="5" t="s">
+        <v>2550</v>
+      </c>
+      <c r="C904" s="3" t="s">
+        <v>2549</v>
+      </c>
+    </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A910" s="7"/>
     </row>

</xml_diff>

<commit_message>
fix techno attachment in buildings, support attach file to launcher
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA7B0AE-1790-4255-8E20-1D2EF5FBA30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC008B44-8D5E-4349-9AEA-DC1579F18CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="31590" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2706" uniqueCount="2551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="2554">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -22127,6 +22127,16 @@
   <si>
     <t>为没有图像的附加单位显示缺省图像</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>将%s文件的默认程序设为FA2</t>
+  </si>
+  <si>
+    <t>Options.BindFormat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set FA2 as the default program for %s files</t>
   </si>
 </sst>
 </file>
@@ -22546,7 +22556,7 @@
   <dimension ref="A1:C917"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A894" workbookViewId="0">
-      <selection activeCell="C904" sqref="A904:C904"/>
+      <selection activeCell="C905" sqref="C905"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -32483,6 +32493,17 @@
         <v>2549</v>
       </c>
     </row>
+    <row r="905" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A905" s="4" t="s">
+        <v>2552</v>
+      </c>
+      <c r="B905" s="5" t="s">
+        <v>2551</v>
+      </c>
+      <c r="C905" s="3" t="s">
+        <v>2553</v>
+      </c>
+    </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A910" s="7"/>
     </row>

</xml_diff>